<commit_message>
updating week 3 ratings with bug fix
</commit_message>
<xml_diff>
--- a/PEAR/PEAR Football/y2025/Spreads/spreads_tracker_week3.xlsx
+++ b/PEAR/PEAR Football/y2025/Spreads/spreads_tracker_week3.xlsx
@@ -511,40 +511,40 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>UCLA</t>
+          <t>Kent State</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>New Mexico</t>
+          <t>Buffalo</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>3</v>
+        <v>2.2</v>
       </c>
       <c r="E2" t="n">
-        <v>8.199999999999999</v>
+        <v>11.4</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>UCLA -14.5</t>
+          <t>Buffalo -22.5</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>UCLA -14.5</t>
+          <t>Buffalo -23.5</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>UCLA -22.7</t>
+          <t>Buffalo -12.1</t>
         </is>
       </c>
       <c r="I2" t="n">
-        <v>22.7</v>
+        <v>-12.1</v>
       </c>
       <c r="J2" t="n">
-        <v>14.5</v>
+        <v>-23.5</v>
       </c>
       <c r="K2" t="inlineStr"/>
       <c r="L2" t="inlineStr"/>
@@ -558,40 +558,40 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Arizona</t>
+          <t>Ohio State</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Kansas State</t>
+          <t>Ohio</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>8.9</v>
+        <v>4.7</v>
       </c>
       <c r="E3" t="n">
-        <v>5.9</v>
+        <v>10.6</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Kansas State -1.5</t>
+          <t>Ohio State -25.5</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Kansas State -1.5</t>
+          <t>Ohio State -25.5</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Arizona -4.4</t>
+          <t>Ohio State -36.1</t>
         </is>
       </c>
       <c r="I3" t="n">
-        <v>4.4</v>
+        <v>36.1</v>
       </c>
       <c r="J3" t="n">
-        <v>-1.5</v>
+        <v>25.5</v>
       </c>
       <c r="K3" t="inlineStr"/>
       <c r="L3" t="inlineStr"/>
@@ -605,40 +605,40 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Tennessee</t>
+          <t>Michigan</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Georgia</t>
+          <t>Central Michigan</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>9.6</v>
+        <v>2.5</v>
       </c>
       <c r="E4" t="n">
-        <v>3.2</v>
+        <v>8.299999999999997</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Georgia -7.5</t>
+          <t>Michigan -27.5</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Georgia -7.5</t>
+          <t>Michigan -27.5</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>Georgia -4.3</t>
+          <t>Michigan -35.8</t>
         </is>
       </c>
       <c r="I4" t="n">
-        <v>-4.3</v>
+        <v>35.8</v>
       </c>
       <c r="J4" t="n">
-        <v>-7.5</v>
+        <v>27.5</v>
       </c>
       <c r="K4" t="inlineStr"/>
       <c r="L4" t="inlineStr"/>
@@ -652,40 +652,40 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Wake Forest</t>
+          <t>Tulsa</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>NC State</t>
+          <t>Navy</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>7.1</v>
+        <v>4.7</v>
       </c>
       <c r="E5" t="n">
-        <v>3</v>
+        <v>7.9</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>NC State -7.5</t>
+          <t>Navy -14.5</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>NC State -7.5</t>
+          <t>Navy -14.5</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>NC State -4.5</t>
+          <t>Navy -6.6</t>
         </is>
       </c>
       <c r="I5" t="n">
-        <v>-4.5</v>
+        <v>-6.6</v>
       </c>
       <c r="J5" t="n">
-        <v>-7.5</v>
+        <v>-14.5</v>
       </c>
       <c r="K5" t="inlineStr"/>
       <c r="L5" t="inlineStr"/>
@@ -699,40 +699,40 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Houston</t>
+          <t>Utah State</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Colorado</t>
+          <t>Air Force</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>8.199999999999999</v>
+        <v>6.6</v>
       </c>
       <c r="E6" t="n">
-        <v>2.8</v>
+        <v>7.4</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Houston -3.5</t>
+          <t>Air Force -3.5</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>Houston -4.5</t>
+          <t>Air Force -3.5</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>Houston -1.7</t>
+          <t>Utah State -3.9</t>
         </is>
       </c>
       <c r="I6" t="n">
-        <v>1.7</v>
+        <v>3.9</v>
       </c>
       <c r="J6" t="n">
-        <v>4.5</v>
+        <v>-3.5</v>
       </c>
       <c r="K6" t="inlineStr"/>
       <c r="L6" t="inlineStr"/>
@@ -746,40 +746,40 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Georgia Tech</t>
+          <t>UAB</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Clemson</t>
+          <t>Akron</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>8.800000000000001</v>
+        <v>3</v>
       </c>
       <c r="E7" t="n">
-        <v>2.1</v>
+        <v>7.399999999999999</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Clemson -8.5</t>
+          <t>UAB -11.5</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>Clemson -8.5</t>
+          <t>UAB -11.5</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>Clemson -6.4</t>
+          <t>UAB -18.9</t>
         </is>
       </c>
       <c r="I7" t="n">
-        <v>-6.4</v>
+        <v>18.9</v>
       </c>
       <c r="J7" t="n">
-        <v>-8.5</v>
+        <v>11.5</v>
       </c>
       <c r="K7" t="inlineStr"/>
       <c r="L7" t="inlineStr"/>
@@ -793,40 +793,40 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Notre Dame</t>
+          <t>Wyoming</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Texas A&amp;M</t>
+          <t>Utah</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>9.800000000000001</v>
+        <v>4.6</v>
       </c>
       <c r="E8" t="n">
-        <v>1.6</v>
+        <v>7.300000000000001</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Notre Dame -7.0</t>
+          <t>Utah -22.5</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>Notre Dame -7</t>
+          <t>Utah -22.5</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>Notre Dame -8.6</t>
+          <t>Utah -15.2</t>
         </is>
       </c>
       <c r="I8" t="n">
-        <v>8.6</v>
+        <v>-15.2</v>
       </c>
       <c r="J8" t="n">
-        <v>7</v>
+        <v>-22.5</v>
       </c>
       <c r="K8" t="inlineStr"/>
       <c r="L8" t="inlineStr"/>
@@ -840,40 +840,40 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>West Virginia</t>
+          <t>Temple</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Pittsburgh</t>
+          <t>Oklahoma</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>7.9</v>
+        <v>5.4</v>
       </c>
       <c r="E9" t="n">
-        <v>1.1</v>
+        <v>6.399999999999999</v>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Pittsburgh -2.5</t>
+          <t>Oklahoma -25.5</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>Pittsburgh -2.5</t>
+          <t>Oklahoma -24.5</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>Pittsburgh -3.6</t>
+          <t>Oklahoma -18.1</t>
         </is>
       </c>
       <c r="I9" t="n">
-        <v>-3.6</v>
+        <v>-18.1</v>
       </c>
       <c r="J9" t="n">
-        <v>-2.5</v>
+        <v>-24.5</v>
       </c>
       <c r="K9" t="inlineStr"/>
       <c r="L9" t="inlineStr"/>
@@ -887,40 +887,40 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>LSU</t>
+          <t>Arkansas State</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Florida</t>
+          <t>Iowa State</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>9.800000000000001</v>
+        <v>3.7</v>
       </c>
       <c r="E10" t="n">
-        <v>0.7999999999999998</v>
+        <v>5.9</v>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>LSU -5.5</t>
+          <t>Iowa State -21.5</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>LSU -5.5</t>
+          <t>Iowa State -21.5</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>LSU -6.3</t>
+          <t>Iowa State -15.6</t>
         </is>
       </c>
       <c r="I10" t="n">
-        <v>6.3</v>
+        <v>-15.6</v>
       </c>
       <c r="J10" t="n">
-        <v>5.5</v>
+        <v>-21.5</v>
       </c>
       <c r="K10" t="inlineStr"/>
       <c r="L10" t="inlineStr"/>
@@ -934,33 +934,41 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Texas</t>
+          <t>Auburn</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>UTEP</t>
+          <t>South Alabama</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>3.4</v>
-      </c>
-      <c r="E11" t="inlineStr"/>
+        <v>6.2</v>
+      </c>
+      <c r="E11" t="n">
+        <v>5.699999999999999</v>
+      </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Texas -nan</t>
-        </is>
-      </c>
-      <c r="G11" t="inlineStr"/>
+          <t>Auburn -25.5</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>Auburn -25.5</t>
+        </is>
+      </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>Texas -37.5</t>
+          <t>Auburn -19.8</t>
         </is>
       </c>
       <c r="I11" t="n">
-        <v>37.5</v>
-      </c>
-      <c r="J11" t="inlineStr"/>
+        <v>19.8</v>
+      </c>
+      <c r="J11" t="n">
+        <v>25.5</v>
+      </c>
       <c r="K11" t="inlineStr"/>
       <c r="L11" t="inlineStr"/>
       <c r="M11" t="inlineStr"/>
@@ -973,33 +981,41 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Iowa</t>
+          <t>Missouri</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Massachusetts</t>
+          <t>Louisiana</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>3.7</v>
-      </c>
-      <c r="E12" t="inlineStr"/>
+        <v>6.9</v>
+      </c>
+      <c r="E12" t="n">
+        <v>5.600000000000001</v>
+      </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>Iowa -nan</t>
-        </is>
-      </c>
-      <c r="G12" t="inlineStr"/>
+          <t>Missouri -22.5</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>Missouri -24.5</t>
+        </is>
+      </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>Iowa -24.2</t>
+          <t>Missouri -18.9</t>
         </is>
       </c>
       <c r="I12" t="n">
-        <v>24.2</v>
-      </c>
-      <c r="J12" t="inlineStr"/>
+        <v>18.9</v>
+      </c>
+      <c r="J12" t="n">
+        <v>24.5</v>
+      </c>
       <c r="K12" t="inlineStr"/>
       <c r="L12" t="inlineStr"/>
       <c r="M12" t="inlineStr"/>
@@ -1012,33 +1028,41 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Michigan</t>
+          <t>Northwestern</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Central Michigan</t>
+          <t>Oregon</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>2.5</v>
-      </c>
-      <c r="E13" t="inlineStr"/>
+        <v>5.8</v>
+      </c>
+      <c r="E13" t="n">
+        <v>5.399999999999999</v>
+      </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>Michigan -nan</t>
-        </is>
-      </c>
-      <c r="G13" t="inlineStr"/>
+          <t>Oregon -27.5</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>Oregon -27.5</t>
+        </is>
+      </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>Michigan -35.8</t>
+          <t>Oregon -22.1</t>
         </is>
       </c>
       <c r="I13" t="n">
-        <v>35.8</v>
-      </c>
-      <c r="J13" t="inlineStr"/>
+        <v>-22.1</v>
+      </c>
+      <c r="J13" t="n">
+        <v>-27.5</v>
+      </c>
       <c r="K13" t="inlineStr"/>
       <c r="L13" t="inlineStr"/>
       <c r="M13" t="inlineStr"/>
@@ -1051,33 +1075,41 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Ohio State</t>
+          <t>Purdue</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Ohio</t>
+          <t>USC</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>4.7</v>
-      </c>
-      <c r="E14" t="inlineStr"/>
+        <v>6.4</v>
+      </c>
+      <c r="E14" t="n">
+        <v>5.300000000000001</v>
+      </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>Ohio State -nan</t>
-        </is>
-      </c>
-      <c r="G14" t="inlineStr"/>
+          <t>USC -21.5</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>USC -21.5</t>
+        </is>
+      </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>Ohio State -36.1</t>
+          <t>USC -16.2</t>
         </is>
       </c>
       <c r="I14" t="n">
-        <v>36.1</v>
-      </c>
-      <c r="J14" t="inlineStr"/>
+        <v>-16.2</v>
+      </c>
+      <c r="J14" t="n">
+        <v>-21.5</v>
+      </c>
       <c r="K14" t="inlineStr"/>
       <c r="L14" t="inlineStr"/>
       <c r="M14" t="inlineStr"/>
@@ -1090,33 +1122,41 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Illinois</t>
+          <t>Arizona State</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Western Michigan</t>
+          <t>Texas State</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>3.3</v>
-      </c>
-      <c r="E15" t="inlineStr"/>
+        <v>8.300000000000001</v>
+      </c>
+      <c r="E15" t="n">
+        <v>4.9</v>
+      </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>Illinois -nan</t>
-        </is>
-      </c>
-      <c r="G15" t="inlineStr"/>
+          <t>Arizona State -14.5</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>Arizona State -14.5</t>
+        </is>
+      </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>Illinois -26.5</t>
+          <t>Arizona State -9.6</t>
         </is>
       </c>
       <c r="I15" t="n">
-        <v>26.5</v>
-      </c>
-      <c r="J15" t="inlineStr"/>
+        <v>9.6</v>
+      </c>
+      <c r="J15" t="n">
+        <v>14.5</v>
+      </c>
       <c r="K15" t="inlineStr"/>
       <c r="L15" t="inlineStr"/>
       <c r="M15" t="inlineStr"/>
@@ -1129,33 +1169,41 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Alabama</t>
+          <t>Nevada</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Wisconsin</t>
+          <t>Middle Tennessee</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>8.1</v>
-      </c>
-      <c r="E16" t="inlineStr"/>
+        <v>5.6</v>
+      </c>
+      <c r="E16" t="n">
+        <v>4.1</v>
+      </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>Alabama -nan</t>
-        </is>
-      </c>
-      <c r="G16" t="inlineStr"/>
+          <t>Nevada -9.5</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>Nevada -8.5</t>
+        </is>
+      </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>Alabama -23.8</t>
+          <t>Nevada -4.4</t>
         </is>
       </c>
       <c r="I16" t="n">
-        <v>23.8</v>
-      </c>
-      <c r="J16" t="inlineStr"/>
+        <v>4.4</v>
+      </c>
+      <c r="J16" t="n">
+        <v>8.5</v>
+      </c>
       <c r="K16" t="inlineStr"/>
       <c r="L16" t="inlineStr"/>
       <c r="M16" t="inlineStr"/>
@@ -1168,33 +1216,41 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Kentucky</t>
+          <t>Tulane</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Eastern Michigan</t>
+          <t>Duke</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>3.8</v>
-      </c>
-      <c r="E17" t="inlineStr"/>
+        <v>8.300000000000001</v>
+      </c>
+      <c r="E17" t="n">
+        <v>3.9</v>
+      </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>Kentucky -nan</t>
-        </is>
-      </c>
-      <c r="G17" t="inlineStr"/>
+          <t>Tulane -2.5</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>Tulane -2.5</t>
+        </is>
+      </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>Kentucky -22.1</t>
+          <t>Tulane -6.4</t>
         </is>
       </c>
       <c r="I17" t="n">
-        <v>22.1</v>
-      </c>
-      <c r="J17" t="inlineStr"/>
+        <v>6.4</v>
+      </c>
+      <c r="J17" t="n">
+        <v>2.5</v>
+      </c>
       <c r="K17" t="inlineStr"/>
       <c r="L17" t="inlineStr"/>
       <c r="M17" t="inlineStr"/>
@@ -1207,33 +1263,41 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Texas Tech</t>
+          <t>UCLA</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Oregon State</t>
+          <t>New Mexico</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>7.5</v>
-      </c>
-      <c r="E18" t="inlineStr"/>
+        <v>3.3</v>
+      </c>
+      <c r="E18" t="n">
+        <v>3.800000000000001</v>
+      </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>Texas Tech -nan</t>
-        </is>
-      </c>
-      <c r="G18" t="inlineStr"/>
+          <t>UCLA -14.5</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>UCLA -14.5</t>
+        </is>
+      </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>Texas Tech -16.8</t>
+          <t>UCLA -18.3</t>
         </is>
       </c>
       <c r="I18" t="n">
-        <v>16.8</v>
-      </c>
-      <c r="J18" t="inlineStr"/>
+        <v>18.3</v>
+      </c>
+      <c r="J18" t="n">
+        <v>14.5</v>
+      </c>
       <c r="K18" t="inlineStr"/>
       <c r="L18" t="inlineStr"/>
       <c r="M18" t="inlineStr"/>
@@ -1246,33 +1310,41 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>UAB</t>
+          <t>Stanford</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Akron</t>
+          <t>Boston College</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>3</v>
-      </c>
-      <c r="E19" t="inlineStr"/>
+        <v>6.3</v>
+      </c>
+      <c r="E19" t="n">
+        <v>3.8</v>
+      </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>UAB -nan</t>
-        </is>
-      </c>
-      <c r="G19" t="inlineStr"/>
+          <t>Boston College -10.5</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>Boston College -10.5</t>
+        </is>
+      </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>UAB -18.9</t>
+          <t>Boston College -6.7</t>
         </is>
       </c>
       <c r="I19" t="n">
-        <v>18.9</v>
-      </c>
-      <c r="J19" t="inlineStr"/>
+        <v>-6.7</v>
+      </c>
+      <c r="J19" t="n">
+        <v>-10.5</v>
+      </c>
       <c r="K19" t="inlineStr"/>
       <c r="L19" t="inlineStr"/>
       <c r="M19" t="inlineStr"/>
@@ -1285,33 +1357,41 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Ole Miss</t>
+          <t>Virginia Tech</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Arkansas</t>
+          <t>Old Dominion</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>9.4</v>
-      </c>
-      <c r="E20" t="inlineStr"/>
+        <v>6.9</v>
+      </c>
+      <c r="E20" t="n">
+        <v>3.6</v>
+      </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>Ole Miss -nan</t>
-        </is>
-      </c>
-      <c r="G20" t="inlineStr"/>
+          <t>Virginia Tech -6.5</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>Virginia Tech -7.5</t>
+        </is>
+      </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>Ole Miss -7.8</t>
+          <t>Virginia Tech -11.1</t>
         </is>
       </c>
       <c r="I20" t="n">
-        <v>7.8</v>
-      </c>
-      <c r="J20" t="inlineStr"/>
+        <v>11.1</v>
+      </c>
+      <c r="J20" t="n">
+        <v>7.5</v>
+      </c>
       <c r="K20" t="inlineStr"/>
       <c r="L20" t="inlineStr"/>
       <c r="M20" t="inlineStr"/>
@@ -1324,33 +1404,41 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Missouri</t>
+          <t>Kentucky</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Louisiana</t>
+          <t>Eastern Michigan</t>
         </is>
       </c>
       <c r="D21" t="n">
-        <v>6.9</v>
-      </c>
-      <c r="E21" t="inlineStr"/>
+        <v>3.8</v>
+      </c>
+      <c r="E21" t="n">
+        <v>3.399999999999999</v>
+      </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>Missouri -nan</t>
-        </is>
-      </c>
-      <c r="G21" t="inlineStr"/>
+          <t>Kentucky -25.5</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>Kentucky -25.5</t>
+        </is>
+      </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>Missouri -18.9</t>
+          <t>Kentucky -22.1</t>
         </is>
       </c>
       <c r="I21" t="n">
-        <v>18.9</v>
-      </c>
-      <c r="J21" t="inlineStr"/>
+        <v>22.1</v>
+      </c>
+      <c r="J21" t="n">
+        <v>25.5</v>
+      </c>
       <c r="K21" t="inlineStr"/>
       <c r="L21" t="inlineStr"/>
       <c r="M21" t="inlineStr"/>
@@ -1363,33 +1451,41 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Tulane</t>
+          <t>Alabama</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Duke</t>
+          <t>Wisconsin</t>
         </is>
       </c>
       <c r="D22" t="n">
-        <v>8.300000000000001</v>
-      </c>
-      <c r="E22" t="inlineStr"/>
+        <v>8.1</v>
+      </c>
+      <c r="E22" t="n">
+        <v>3.300000000000001</v>
+      </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>Tulane -nan</t>
-        </is>
-      </c>
-      <c r="G22" t="inlineStr"/>
+          <t>Alabama -22.5</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>Alabama -20.5</t>
+        </is>
+      </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>Tulane -6.4</t>
+          <t>Alabama -23.8</t>
         </is>
       </c>
       <c r="I22" t="n">
-        <v>6.4</v>
-      </c>
-      <c r="J22" t="inlineStr"/>
+        <v>23.8</v>
+      </c>
+      <c r="J22" t="n">
+        <v>20.5</v>
+      </c>
       <c r="K22" t="inlineStr"/>
       <c r="L22" t="inlineStr"/>
       <c r="M22" t="inlineStr"/>
@@ -1402,33 +1498,41 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Miami</t>
+          <t>Tennessee</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>South Florida</t>
+          <t>Georgia</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>7.9</v>
-      </c>
-      <c r="E23" t="inlineStr"/>
+        <v>9.6</v>
+      </c>
+      <c r="E23" t="n">
+        <v>3.2</v>
+      </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>Miami -nan</t>
-        </is>
-      </c>
-      <c r="G23" t="inlineStr"/>
+          <t>Georgia -7.5</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>Georgia -7.5</t>
+        </is>
+      </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>Miami -18.3</t>
+          <t>Georgia -4.3</t>
         </is>
       </c>
       <c r="I23" t="n">
-        <v>18.3</v>
-      </c>
-      <c r="J23" t="inlineStr"/>
+        <v>-4.3</v>
+      </c>
+      <c r="J23" t="n">
+        <v>-7.5</v>
+      </c>
       <c r="K23" t="inlineStr"/>
       <c r="L23" t="inlineStr"/>
       <c r="M23" t="inlineStr"/>
@@ -1441,33 +1545,41 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>South Carolina</t>
+          <t>Wake Forest</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Vanderbilt</t>
+          <t>NC State</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>9.199999999999999</v>
-      </c>
-      <c r="E24" t="inlineStr"/>
+        <v>7.1</v>
+      </c>
+      <c r="E24" t="n">
+        <v>3</v>
+      </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>South Carolina -nan</t>
-        </is>
-      </c>
-      <c r="G24" t="inlineStr"/>
+          <t>NC State -7.5</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>NC State -7.5</t>
+        </is>
+      </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>South Carolina -8.2</t>
+          <t>NC State -4.5</t>
         </is>
       </c>
       <c r="I24" t="n">
-        <v>8.199999999999999</v>
-      </c>
-      <c r="J24" t="inlineStr"/>
+        <v>-4.5</v>
+      </c>
+      <c r="J24" t="n">
+        <v>-7.5</v>
+      </c>
       <c r="K24" t="inlineStr"/>
       <c r="L24" t="inlineStr"/>
       <c r="M24" t="inlineStr"/>
@@ -1480,33 +1592,41 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Louisiana Tech</t>
+          <t>Arizona</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>New Mexico State</t>
+          <t>Kansas State</t>
         </is>
       </c>
       <c r="D25" t="n">
-        <v>4.2</v>
-      </c>
-      <c r="E25" t="inlineStr"/>
+        <v>8.9</v>
+      </c>
+      <c r="E25" t="n">
+        <v>2.9</v>
+      </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>Louisiana Tech -nan</t>
-        </is>
-      </c>
-      <c r="G25" t="inlineStr"/>
+          <t>Kansas State -1.5</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>Arizona -1.5</t>
+        </is>
+      </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>Louisiana Tech -9.7</t>
+          <t>Arizona -4.4</t>
         </is>
       </c>
       <c r="I25" t="n">
-        <v>9.699999999999999</v>
-      </c>
-      <c r="J25" t="inlineStr"/>
+        <v>4.4</v>
+      </c>
+      <c r="J25" t="n">
+        <v>1.5</v>
+      </c>
       <c r="K25" t="inlineStr"/>
       <c r="L25" t="inlineStr"/>
       <c r="M25" t="inlineStr"/>
@@ -1519,33 +1639,41 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Florida International</t>
+          <t>North Texas</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Florida Atlantic</t>
+          <t>Washington State</t>
         </is>
       </c>
       <c r="D26" t="n">
-        <v>6.7</v>
-      </c>
-      <c r="E26" t="inlineStr"/>
+        <v>7.7</v>
+      </c>
+      <c r="E26" t="n">
+        <v>2.9</v>
+      </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>Florida International -nan</t>
-        </is>
-      </c>
-      <c r="G26" t="inlineStr"/>
+          <t>North Texas -5.5</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>North Texas -5.5</t>
+        </is>
+      </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>Florida International -4.1</t>
+          <t>North Texas -2.6</t>
         </is>
       </c>
       <c r="I26" t="n">
-        <v>4.1</v>
-      </c>
-      <c r="J26" t="inlineStr"/>
+        <v>2.6</v>
+      </c>
+      <c r="J26" t="n">
+        <v>5.5</v>
+      </c>
       <c r="K26" t="inlineStr"/>
       <c r="L26" t="inlineStr"/>
       <c r="M26" t="inlineStr"/>
@@ -1558,33 +1686,41 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Auburn</t>
+          <t>Iowa</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>South Alabama</t>
+          <t>Massachusetts</t>
         </is>
       </c>
       <c r="D27" t="n">
-        <v>6.2</v>
-      </c>
-      <c r="E27" t="inlineStr"/>
+        <v>2.3</v>
+      </c>
+      <c r="E27" t="n">
+        <v>2.899999999999999</v>
+      </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>Auburn -nan</t>
-        </is>
-      </c>
-      <c r="G27" t="inlineStr"/>
+          <t>Iowa -33.5</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>Iowa -33.5</t>
+        </is>
+      </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>Auburn -19.8</t>
+          <t>Iowa -30.6</t>
         </is>
       </c>
       <c r="I27" t="n">
-        <v>19.8</v>
-      </c>
-      <c r="J27" t="inlineStr"/>
+        <v>30.6</v>
+      </c>
+      <c r="J27" t="n">
+        <v>33.5</v>
+      </c>
       <c r="K27" t="inlineStr"/>
       <c r="L27" t="inlineStr"/>
       <c r="M27" t="inlineStr"/>
@@ -1597,33 +1733,41 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Nevada</t>
+          <t>Miami</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Middle Tennessee</t>
+          <t>South Florida</t>
         </is>
       </c>
       <c r="D28" t="n">
-        <v>5.6</v>
-      </c>
-      <c r="E28" t="inlineStr"/>
+        <v>7.9</v>
+      </c>
+      <c r="E28" t="n">
+        <v>2.800000000000001</v>
+      </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>Nevada -nan</t>
-        </is>
-      </c>
-      <c r="G28" t="inlineStr"/>
+          <t>Miami -15.5</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>Miami -15.5</t>
+        </is>
+      </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>Nevada -4.4</t>
+          <t>Miami -18.3</t>
         </is>
       </c>
       <c r="I28" t="n">
-        <v>4.4</v>
-      </c>
-      <c r="J28" t="inlineStr"/>
+        <v>18.3</v>
+      </c>
+      <c r="J28" t="n">
+        <v>15.5</v>
+      </c>
       <c r="K28" t="inlineStr"/>
       <c r="L28" t="inlineStr"/>
       <c r="M28" t="inlineStr"/>
@@ -1636,33 +1780,41 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Arizona State</t>
+          <t>Louisiana Tech</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Texas State</t>
+          <t>New Mexico State</t>
         </is>
       </c>
       <c r="D29" t="n">
-        <v>8.300000000000001</v>
-      </c>
-      <c r="E29" t="inlineStr"/>
+        <v>4.2</v>
+      </c>
+      <c r="E29" t="n">
+        <v>2.800000000000001</v>
+      </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>Arizona State -nan</t>
-        </is>
-      </c>
-      <c r="G29" t="inlineStr"/>
+          <t>Louisiana Tech -12.5</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>Louisiana Tech -12.5</t>
+        </is>
+      </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>Arizona State -9.6</t>
+          <t>Louisiana Tech -9.7</t>
         </is>
       </c>
       <c r="I29" t="n">
-        <v>9.6</v>
-      </c>
-      <c r="J29" t="inlineStr"/>
+        <v>9.699999999999999</v>
+      </c>
+      <c r="J29" t="n">
+        <v>12.5</v>
+      </c>
       <c r="K29" t="inlineStr"/>
       <c r="L29" t="inlineStr"/>
       <c r="M29" t="inlineStr"/>
@@ -1675,33 +1827,41 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Virginia Tech</t>
+          <t>Houston</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Old Dominion</t>
+          <t>Colorado</t>
         </is>
       </c>
       <c r="D30" t="n">
-        <v>6.9</v>
-      </c>
-      <c r="E30" t="inlineStr"/>
+        <v>8.199999999999999</v>
+      </c>
+      <c r="E30" t="n">
+        <v>2.8</v>
+      </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>Virginia Tech -nan</t>
-        </is>
-      </c>
-      <c r="G30" t="inlineStr"/>
+          <t>Houston -3.5</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>Houston -4.5</t>
+        </is>
+      </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>Virginia Tech -11.1</t>
+          <t>Houston -1.7</t>
         </is>
       </c>
       <c r="I30" t="n">
-        <v>11.1</v>
-      </c>
-      <c r="J30" t="inlineStr"/>
+        <v>1.7</v>
+      </c>
+      <c r="J30" t="n">
+        <v>4.5</v>
+      </c>
       <c r="K30" t="inlineStr"/>
       <c r="L30" t="inlineStr"/>
       <c r="M30" t="inlineStr"/>
@@ -1714,33 +1874,41 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Delaware</t>
+          <t>South Carolina</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>UConn</t>
+          <t>Vanderbilt</t>
         </is>
       </c>
       <c r="D31" t="n">
-        <v>3.4</v>
-      </c>
-      <c r="E31" t="inlineStr"/>
+        <v>9.199999999999999</v>
+      </c>
+      <c r="E31" t="n">
+        <v>2.699999999999999</v>
+      </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>Delaware -nan</t>
-        </is>
-      </c>
-      <c r="G31" t="inlineStr"/>
+          <t>South Carolina -5.5</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>South Carolina -5.5</t>
+        </is>
+      </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>UConn -7.7</t>
+          <t>South Carolina -8.2</t>
         </is>
       </c>
       <c r="I31" t="n">
-        <v>-7.7</v>
-      </c>
-      <c r="J31" t="inlineStr"/>
+        <v>8.199999999999999</v>
+      </c>
+      <c r="J31" t="n">
+        <v>5.5</v>
+      </c>
       <c r="K31" t="inlineStr"/>
       <c r="L31" t="inlineStr"/>
       <c r="M31" t="inlineStr"/>
@@ -1753,33 +1921,41 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Utah State</t>
+          <t>Georgia Tech</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Air Force</t>
+          <t>Clemson</t>
         </is>
       </c>
       <c r="D32" t="n">
-        <v>6.6</v>
-      </c>
-      <c r="E32" t="inlineStr"/>
+        <v>8.800000000000001</v>
+      </c>
+      <c r="E32" t="n">
+        <v>2.1</v>
+      </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>Utah State -nan</t>
-        </is>
-      </c>
-      <c r="G32" t="inlineStr"/>
+          <t>Clemson -8.5</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>Clemson -8.5</t>
+        </is>
+      </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>Utah State -3.9</t>
+          <t>Clemson -6.4</t>
         </is>
       </c>
       <c r="I32" t="n">
-        <v>3.9</v>
-      </c>
-      <c r="J32" t="inlineStr"/>
+        <v>-6.4</v>
+      </c>
+      <c r="J32" t="n">
+        <v>-8.5</v>
+      </c>
       <c r="K32" t="inlineStr"/>
       <c r="L32" t="inlineStr"/>
       <c r="M32" t="inlineStr"/>
@@ -1792,33 +1968,41 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Bowling Green</t>
+          <t>Illinois</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Liberty</t>
+          <t>Western Michigan</t>
         </is>
       </c>
       <c r="D33" t="n">
-        <v>4.8</v>
-      </c>
-      <c r="E33" t="inlineStr"/>
+        <v>3.3</v>
+      </c>
+      <c r="E33" t="n">
+        <v>2</v>
+      </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>Bowling Green -nan</t>
-        </is>
-      </c>
-      <c r="G33" t="inlineStr"/>
+          <t>Illinois -28.5</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>Illinois -28.5</t>
+        </is>
+      </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>Liberty -6.4</t>
+          <t>Illinois -26.5</t>
         </is>
       </c>
       <c r="I33" t="n">
-        <v>-6.4</v>
-      </c>
-      <c r="J33" t="inlineStr"/>
+        <v>26.5</v>
+      </c>
+      <c r="J33" t="n">
+        <v>28.5</v>
+      </c>
       <c r="K33" t="inlineStr"/>
       <c r="L33" t="inlineStr"/>
       <c r="M33" t="inlineStr"/>
@@ -1831,33 +2015,41 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>California</t>
+          <t>Delaware</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Minnesota</t>
+          <t>UConn</t>
         </is>
       </c>
       <c r="D34" t="n">
-        <v>8</v>
-      </c>
-      <c r="E34" t="inlineStr"/>
+        <v>3.4</v>
+      </c>
+      <c r="E34" t="n">
+        <v>1.8</v>
+      </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>California -nan</t>
-        </is>
-      </c>
-      <c r="G34" t="inlineStr"/>
+          <t>UConn -10.5</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>UConn -9.5</t>
+        </is>
+      </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>Minnesota -1.9</t>
+          <t>UConn -7.7</t>
         </is>
       </c>
       <c r="I34" t="n">
-        <v>-1.9</v>
-      </c>
-      <c r="J34" t="inlineStr"/>
+        <v>-7.7</v>
+      </c>
+      <c r="J34" t="n">
+        <v>-9.5</v>
+      </c>
       <c r="K34" t="inlineStr"/>
       <c r="L34" t="inlineStr"/>
       <c r="M34" t="inlineStr"/>
@@ -1870,33 +2062,41 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>North Texas</t>
+          <t>Ole Miss</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Washington State</t>
+          <t>Arkansas</t>
         </is>
       </c>
       <c r="D35" t="n">
-        <v>7.7</v>
-      </c>
-      <c r="E35" t="inlineStr"/>
+        <v>9.4</v>
+      </c>
+      <c r="E35" t="n">
+        <v>1.7</v>
+      </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>North Texas -nan</t>
-        </is>
-      </c>
-      <c r="G35" t="inlineStr"/>
+          <t>Ole Miss -8.5</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>Ole Miss -9.5</t>
+        </is>
+      </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>North Texas -2.6</t>
+          <t>Ole Miss -7.8</t>
         </is>
       </c>
       <c r="I35" t="n">
-        <v>2.6</v>
-      </c>
-      <c r="J35" t="inlineStr"/>
+        <v>7.8</v>
+      </c>
+      <c r="J35" t="n">
+        <v>9.5</v>
+      </c>
       <c r="K35" t="inlineStr"/>
       <c r="L35" t="inlineStr"/>
       <c r="M35" t="inlineStr"/>
@@ -1909,33 +2109,41 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Troy</t>
+          <t>Notre Dame</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Memphis</t>
+          <t>Texas A&amp;M</t>
         </is>
       </c>
       <c r="D36" t="n">
-        <v>6.5</v>
-      </c>
-      <c r="E36" t="inlineStr"/>
+        <v>9.800000000000001</v>
+      </c>
+      <c r="E36" t="n">
+        <v>1.6</v>
+      </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>Troy -nan</t>
-        </is>
-      </c>
-      <c r="G36" t="inlineStr"/>
+          <t>Notre Dame -7.0</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>Notre Dame -7</t>
+        </is>
+      </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>Memphis -5.3</t>
+          <t>Notre Dame -8.6</t>
         </is>
       </c>
       <c r="I36" t="n">
-        <v>-5.3</v>
-      </c>
-      <c r="J36" t="inlineStr"/>
+        <v>8.6</v>
+      </c>
+      <c r="J36" t="n">
+        <v>7</v>
+      </c>
       <c r="K36" t="inlineStr"/>
       <c r="L36" t="inlineStr"/>
       <c r="M36" t="inlineStr"/>
@@ -1948,33 +2156,41 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Coastal Carolina</t>
+          <t>Florida International</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>East Carolina</t>
+          <t>Florida Atlantic</t>
         </is>
       </c>
       <c r="D37" t="n">
-        <v>7.7</v>
-      </c>
-      <c r="E37" t="inlineStr"/>
+        <v>6.7</v>
+      </c>
+      <c r="E37" t="n">
+        <v>1.6</v>
+      </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>Coastal Carolina -nan</t>
-        </is>
-      </c>
-      <c r="G37" t="inlineStr"/>
+          <t>Florida International -4.5</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>Florida International -2.5</t>
+        </is>
+      </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>Coastal Carolina -2.6</t>
+          <t>Florida International -4.1</t>
         </is>
       </c>
       <c r="I37" t="n">
-        <v>2.6</v>
-      </c>
-      <c r="J37" t="inlineStr"/>
+        <v>4.1</v>
+      </c>
+      <c r="J37" t="n">
+        <v>2.5</v>
+      </c>
       <c r="K37" t="inlineStr"/>
       <c r="L37" t="inlineStr"/>
       <c r="M37" t="inlineStr"/>
@@ -1987,33 +2203,41 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Stanford</t>
+          <t>Texas Tech</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Boston College</t>
+          <t>Oregon State</t>
         </is>
       </c>
       <c r="D38" t="n">
-        <v>6.3</v>
-      </c>
-      <c r="E38" t="inlineStr"/>
+        <v>5.4</v>
+      </c>
+      <c r="E38" t="n">
+        <v>1.300000000000001</v>
+      </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>Stanford -nan</t>
-        </is>
-      </c>
-      <c r="G38" t="inlineStr"/>
+          <t>Texas Tech -24.5</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>Texas Tech -24.5</t>
+        </is>
+      </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>Boston College -6.7</t>
+          <t>Texas Tech -23.2</t>
         </is>
       </c>
       <c r="I38" t="n">
-        <v>-6.7</v>
-      </c>
-      <c r="J38" t="inlineStr"/>
+        <v>23.2</v>
+      </c>
+      <c r="J38" t="n">
+        <v>24.5</v>
+      </c>
       <c r="K38" t="inlineStr"/>
       <c r="L38" t="inlineStr"/>
       <c r="M38" t="inlineStr"/>
@@ -2026,33 +2250,41 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Wyoming</t>
+          <t>Coastal Carolina</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Utah</t>
+          <t>East Carolina</t>
         </is>
       </c>
       <c r="D39" t="n">
-        <v>4.6</v>
-      </c>
-      <c r="E39" t="inlineStr"/>
+        <v>4.4</v>
+      </c>
+      <c r="E39" t="n">
+        <v>1.3</v>
+      </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>Wyoming -nan</t>
-        </is>
-      </c>
-      <c r="G39" t="inlineStr"/>
+          <t>East Carolina -6.5</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>East Carolina -6.5</t>
+        </is>
+      </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>Utah -15.2</t>
+          <t>East Carolina -7.8</t>
         </is>
       </c>
       <c r="I39" t="n">
-        <v>-15.2</v>
-      </c>
-      <c r="J39" t="inlineStr"/>
+        <v>-7.8</v>
+      </c>
+      <c r="J39" t="n">
+        <v>-6.5</v>
+      </c>
       <c r="K39" t="inlineStr"/>
       <c r="L39" t="inlineStr"/>
       <c r="M39" t="inlineStr"/>
@@ -2065,33 +2297,41 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Georgia Southern</t>
+          <t>Troy</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Jacksonville State</t>
+          <t>Memphis</t>
         </is>
       </c>
       <c r="D40" t="n">
-        <v>6.6</v>
-      </c>
-      <c r="E40" t="inlineStr"/>
+        <v>6.5</v>
+      </c>
+      <c r="E40" t="n">
+        <v>1.2</v>
+      </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>Georgia Southern -nan</t>
-        </is>
-      </c>
-      <c r="G40" t="inlineStr"/>
+          <t>Troy -nan</t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>Memphis -6.5</t>
+        </is>
+      </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>Georgia Southern -2.5</t>
+          <t>Memphis -5.3</t>
         </is>
       </c>
       <c r="I40" t="n">
-        <v>2.5</v>
-      </c>
-      <c r="J40" t="inlineStr"/>
+        <v>-5.3</v>
+      </c>
+      <c r="J40" t="n">
+        <v>-6.5</v>
+      </c>
       <c r="K40" t="inlineStr"/>
       <c r="L40" t="inlineStr"/>
       <c r="M40" t="inlineStr"/>
@@ -2104,33 +2344,41 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Missouri State</t>
+          <t>West Virginia</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>SMU</t>
+          <t>Pittsburgh</t>
         </is>
       </c>
       <c r="D41" t="n">
-        <v>2</v>
-      </c>
-      <c r="E41" t="inlineStr"/>
+        <v>7.9</v>
+      </c>
+      <c r="E41" t="n">
+        <v>1.1</v>
+      </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>Missouri State -nan</t>
-        </is>
-      </c>
-      <c r="G41" t="inlineStr"/>
+          <t>Pittsburgh -2.5</t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>Pittsburgh -2.5</t>
+        </is>
+      </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>SMU -28.3</t>
+          <t>Pittsburgh -3.6</t>
         </is>
       </c>
       <c r="I41" t="n">
-        <v>-28.3</v>
-      </c>
-      <c r="J41" t="inlineStr"/>
+        <v>-3.6</v>
+      </c>
+      <c r="J41" t="n">
+        <v>-2.5</v>
+      </c>
       <c r="K41" t="inlineStr"/>
       <c r="L41" t="inlineStr"/>
       <c r="M41" t="inlineStr"/>
@@ -2143,33 +2391,41 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Southern Miss</t>
+          <t>Texas</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>App State</t>
+          <t>UTEP</t>
         </is>
       </c>
       <c r="D42" t="n">
-        <v>5.6</v>
-      </c>
-      <c r="E42" t="inlineStr"/>
+        <v>3.4</v>
+      </c>
+      <c r="E42" t="n">
+        <v>1</v>
+      </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>Southern Miss -nan</t>
-        </is>
-      </c>
-      <c r="G42" t="inlineStr"/>
+          <t>Texas -36.5</t>
+        </is>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>Texas -36.5</t>
+        </is>
+      </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>App State -1.2</t>
+          <t>Texas -37.5</t>
         </is>
       </c>
       <c r="I42" t="n">
-        <v>-1.2</v>
-      </c>
-      <c r="J42" t="inlineStr"/>
+        <v>37.5</v>
+      </c>
+      <c r="J42" t="n">
+        <v>36.5</v>
+      </c>
       <c r="K42" t="inlineStr"/>
       <c r="L42" t="inlineStr"/>
       <c r="M42" t="inlineStr"/>
@@ -2182,33 +2438,41 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Arkansas State</t>
+          <t>Georgia Southern</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Iowa State</t>
+          <t>Jacksonville State</t>
         </is>
       </c>
       <c r="D43" t="n">
-        <v>5.8</v>
-      </c>
-      <c r="E43" t="inlineStr"/>
+        <v>6.6</v>
+      </c>
+      <c r="E43" t="n">
+        <v>1</v>
+      </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>Arkansas State -nan</t>
-        </is>
-      </c>
-      <c r="G43" t="inlineStr"/>
+          <t>Georgia Southern -2.5</t>
+        </is>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>Georgia Southern -3.5</t>
+        </is>
+      </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>Iowa State -9.0</t>
+          <t>Georgia Southern -2.5</t>
         </is>
       </c>
       <c r="I43" t="n">
-        <v>-9</v>
-      </c>
-      <c r="J43" t="inlineStr"/>
+        <v>2.5</v>
+      </c>
+      <c r="J43" t="n">
+        <v>3.5</v>
+      </c>
       <c r="K43" t="inlineStr"/>
       <c r="L43" t="inlineStr"/>
       <c r="M43" t="inlineStr"/>
@@ -2221,33 +2485,41 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Temple</t>
+          <t>Missouri State</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Oklahoma</t>
+          <t>SMU</t>
         </is>
       </c>
       <c r="D44" t="n">
-        <v>5.4</v>
-      </c>
-      <c r="E44" t="inlineStr"/>
+        <v>2</v>
+      </c>
+      <c r="E44" t="n">
+        <v>0.8000000000000007</v>
+      </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>Temple -nan</t>
-        </is>
-      </c>
-      <c r="G44" t="inlineStr"/>
+          <t>SMU -27.5</t>
+        </is>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>SMU -27.5</t>
+        </is>
+      </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>Oklahoma -18.1</t>
+          <t>SMU -28.3</t>
         </is>
       </c>
       <c r="I44" t="n">
-        <v>-18.1</v>
-      </c>
-      <c r="J44" t="inlineStr"/>
+        <v>-28.3</v>
+      </c>
+      <c r="J44" t="n">
+        <v>-27.5</v>
+      </c>
       <c r="K44" t="inlineStr"/>
       <c r="L44" t="inlineStr"/>
       <c r="M44" t="inlineStr"/>
@@ -2260,33 +2532,41 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Kent State</t>
+          <t>LSU</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Buffalo</t>
+          <t>Florida</t>
         </is>
       </c>
       <c r="D45" t="n">
-        <v>2.2</v>
-      </c>
-      <c r="E45" t="inlineStr"/>
+        <v>9.800000000000001</v>
+      </c>
+      <c r="E45" t="n">
+        <v>0.7999999999999998</v>
+      </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>Kent State -nan</t>
-        </is>
-      </c>
-      <c r="G45" t="inlineStr"/>
+          <t>LSU -5.5</t>
+        </is>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>LSU -5.5</t>
+        </is>
+      </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>Buffalo -12.1</t>
+          <t>LSU -6.3</t>
         </is>
       </c>
       <c r="I45" t="n">
-        <v>-12.1</v>
-      </c>
-      <c r="J45" t="inlineStr"/>
+        <v>6.3</v>
+      </c>
+      <c r="J45" t="n">
+        <v>5.5</v>
+      </c>
       <c r="K45" t="inlineStr"/>
       <c r="L45" t="inlineStr"/>
       <c r="M45" t="inlineStr"/>
@@ -2299,33 +2579,41 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Tulsa</t>
+          <t>California</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Navy</t>
+          <t>Minnesota</t>
         </is>
       </c>
       <c r="D46" t="n">
-        <v>7.1</v>
-      </c>
-      <c r="E46" t="inlineStr"/>
+        <v>8</v>
+      </c>
+      <c r="E46" t="n">
+        <v>0.6000000000000001</v>
+      </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>Tulsa -nan</t>
-        </is>
-      </c>
-      <c r="G46" t="inlineStr"/>
+          <t>Minnesota -2.5</t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>Minnesota -2.5</t>
+        </is>
+      </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>Tulsa -0.4</t>
+          <t>Minnesota -1.9</t>
         </is>
       </c>
       <c r="I46" t="n">
-        <v>0.4</v>
-      </c>
-      <c r="J46" t="inlineStr"/>
+        <v>-1.9</v>
+      </c>
+      <c r="J46" t="n">
+        <v>-2.5</v>
+      </c>
       <c r="K46" t="inlineStr"/>
       <c r="L46" t="inlineStr"/>
       <c r="M46" t="inlineStr"/>
@@ -2338,33 +2626,41 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Northwestern</t>
+          <t>Southern Miss</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Oregon</t>
+          <t>App State</t>
         </is>
       </c>
       <c r="D47" t="n">
-        <v>5.8</v>
-      </c>
-      <c r="E47" t="inlineStr"/>
+        <v>5.6</v>
+      </c>
+      <c r="E47" t="n">
+        <v>0.3</v>
+      </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>Northwestern -nan</t>
-        </is>
-      </c>
-      <c r="G47" t="inlineStr"/>
+          <t>Southern Miss -2.5</t>
+        </is>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>App State -1.5</t>
+        </is>
+      </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>Oregon -22.1</t>
+          <t>App State -1.2</t>
         </is>
       </c>
       <c r="I47" t="n">
-        <v>-22.1</v>
-      </c>
-      <c r="J47" t="inlineStr"/>
+        <v>-1.2</v>
+      </c>
+      <c r="J47" t="n">
+        <v>-1.5</v>
+      </c>
       <c r="K47" t="inlineStr"/>
       <c r="L47" t="inlineStr"/>
       <c r="M47" t="inlineStr"/>
@@ -2377,33 +2673,41 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Purdue</t>
+          <t>Bowling Green</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>USC</t>
+          <t>Liberty</t>
         </is>
       </c>
       <c r="D48" t="n">
-        <v>6.4</v>
-      </c>
-      <c r="E48" t="inlineStr"/>
+        <v>4.8</v>
+      </c>
+      <c r="E48" t="n">
+        <v>0.09999999999999964</v>
+      </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>Purdue -nan</t>
-        </is>
-      </c>
-      <c r="G48" t="inlineStr"/>
+          <t>Liberty -7.5</t>
+        </is>
+      </c>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>Liberty -6.5</t>
+        </is>
+      </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>USC -16.2</t>
+          <t>Liberty -6.4</t>
         </is>
       </c>
       <c r="I48" t="n">
-        <v>-16.2</v>
-      </c>
-      <c r="J48" t="inlineStr"/>
+        <v>-6.4</v>
+      </c>
+      <c r="J48" t="n">
+        <v>-6.5</v>
+      </c>
       <c r="K48" t="inlineStr"/>
       <c r="L48" t="inlineStr"/>
       <c r="M48" t="inlineStr"/>

</xml_diff>

<commit_message>
filling out spreads tracker
</commit_message>
<xml_diff>
--- a/PEAR/PEAR Football/y2025/Spreads/spreads_tracker_week3.xlsx
+++ b/PEAR/PEAR Football/y2025/Spreads/spreads_tracker_week3.xlsx
@@ -523,16 +523,16 @@
         <v>2.2</v>
       </c>
       <c r="E2" t="n">
-        <v>9.4</v>
+        <v>11.4</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Buffalo -22.5</t>
+          <t>Kent State -nan</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Buffalo -21.5</t>
+          <t>Buffalo -23.5</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
@@ -544,13 +544,25 @@
         <v>-12.1</v>
       </c>
       <c r="J2" t="n">
-        <v>-21.5</v>
-      </c>
-      <c r="K2" t="inlineStr"/>
-      <c r="L2" t="inlineStr"/>
-      <c r="M2" t="inlineStr"/>
-      <c r="N2" t="inlineStr"/>
-      <c r="O2" t="inlineStr"/>
+        <v>-23.5</v>
+      </c>
+      <c r="K2" t="n">
+        <v>-3</v>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>Buffalo -3</t>
+        </is>
+      </c>
+      <c r="M2" t="n">
+        <v>1</v>
+      </c>
+      <c r="N2" t="n">
+        <v>1</v>
+      </c>
+      <c r="O2" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -558,46 +570,58 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Missouri</t>
+          <t>Wyoming</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Louisiana</t>
+          <t>Utah</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>6.9</v>
+        <v>4.6</v>
       </c>
       <c r="E3" t="n">
-        <v>8.600000000000001</v>
+        <v>9.300000000000001</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Missouri -22.5</t>
+          <t>Wyoming -nan</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Missouri -27.5</t>
+          <t>Utah -24.5</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Missouri -18.9</t>
+          <t>Utah -15.2</t>
         </is>
       </c>
       <c r="I3" t="n">
-        <v>18.9</v>
+        <v>-15.2</v>
       </c>
       <c r="J3" t="n">
-        <v>27.5</v>
-      </c>
-      <c r="K3" t="inlineStr"/>
-      <c r="L3" t="inlineStr"/>
-      <c r="M3" t="inlineStr"/>
-      <c r="N3" t="inlineStr"/>
-      <c r="O3" t="inlineStr"/>
+        <v>-24.5</v>
+      </c>
+      <c r="K3" t="n">
+        <v>-3</v>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>Utah -3</t>
+        </is>
+      </c>
+      <c r="M3" t="n">
+        <v>1</v>
+      </c>
+      <c r="N3" t="n">
+        <v>1</v>
+      </c>
+      <c r="O3" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
@@ -605,46 +629,58 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Wyoming</t>
+          <t>Arizona State</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Utah</t>
+          <t>Texas State</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>4.6</v>
+        <v>8.300000000000001</v>
       </c>
       <c r="E4" t="n">
-        <v>8.300000000000001</v>
+        <v>8.800000000000001</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Utah -22.5</t>
+          <t>Arizona State -nan</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Utah -23.5</t>
+          <t>Arizona State -18.5</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>Utah -15.2</t>
+          <t>Arizona State -9.7</t>
         </is>
       </c>
       <c r="I4" t="n">
-        <v>-15.2</v>
+        <v>9.699999999999999</v>
       </c>
       <c r="J4" t="n">
-        <v>-23.5</v>
-      </c>
-      <c r="K4" t="inlineStr"/>
-      <c r="L4" t="inlineStr"/>
-      <c r="M4" t="inlineStr"/>
-      <c r="N4" t="inlineStr"/>
-      <c r="O4" t="inlineStr"/>
+        <v>18.5</v>
+      </c>
+      <c r="K4" t="n">
+        <v>19</v>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>Arizona State -19</t>
+        </is>
+      </c>
+      <c r="M4" t="n">
+        <v>1</v>
+      </c>
+      <c r="N4" t="n">
+        <v>0</v>
+      </c>
+      <c r="O4" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
@@ -664,34 +700,46 @@
         <v>2.5</v>
       </c>
       <c r="E5" t="n">
-        <v>8.299999999999997</v>
+        <v>8.399999999999999</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
+          <t>Michigan -nan</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
           <t>Michigan -27.5</t>
         </is>
       </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>Michigan -27.5</t>
-        </is>
-      </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>Michigan -35.8</t>
+          <t>Michigan -35.9</t>
         </is>
       </c>
       <c r="I5" t="n">
-        <v>35.8</v>
+        <v>35.9</v>
       </c>
       <c r="J5" t="n">
         <v>27.5</v>
       </c>
-      <c r="K5" t="inlineStr"/>
-      <c r="L5" t="inlineStr"/>
-      <c r="M5" t="inlineStr"/>
-      <c r="N5" t="inlineStr"/>
-      <c r="O5" t="inlineStr"/>
+      <c r="K5" t="n">
+        <v>60</v>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>Michigan -60</t>
+        </is>
+      </c>
+      <c r="M5" t="n">
+        <v>1</v>
+      </c>
+      <c r="N5" t="n">
+        <v>1</v>
+      </c>
+      <c r="O5" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
@@ -699,46 +747,58 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Utah State</t>
+          <t>Missouri</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Air Force</t>
+          <t>Louisiana</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>6.6</v>
+        <v>6.9</v>
       </c>
       <c r="E6" t="n">
-        <v>7.4</v>
+        <v>8.399999999999999</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Air Force -3.5</t>
+          <t>Missouri -27.5</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>Air Force -3.5</t>
+          <t>Missouri -27.5</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>Utah State -3.9</t>
+          <t>Missouri -19.1</t>
         </is>
       </c>
       <c r="I6" t="n">
-        <v>3.9</v>
+        <v>19.1</v>
       </c>
       <c r="J6" t="n">
-        <v>-3.5</v>
-      </c>
-      <c r="K6" t="inlineStr"/>
-      <c r="L6" t="inlineStr"/>
-      <c r="M6" t="inlineStr"/>
-      <c r="N6" t="inlineStr"/>
-      <c r="O6" t="inlineStr"/>
+        <v>27.5</v>
+      </c>
+      <c r="K6" t="n">
+        <v>42</v>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>Missouri -42</t>
+        </is>
+      </c>
+      <c r="M6" t="n">
+        <v>0</v>
+      </c>
+      <c r="N6" t="n">
+        <v>0</v>
+      </c>
+      <c r="O6" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
@@ -746,46 +806,58 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>UAB</t>
+          <t>Utah State</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Akron</t>
+          <t>Air Force</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>3</v>
+        <v>6.6</v>
       </c>
       <c r="E7" t="n">
-        <v>7.399999999999999</v>
+        <v>8</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>UAB -11.5</t>
+          <t>Utah State -nan</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>UAB -11.5</t>
+          <t>Air Force -4</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>UAB -18.9</t>
+          <t>Utah State -4.0</t>
         </is>
       </c>
       <c r="I7" t="n">
-        <v>18.9</v>
+        <v>4</v>
       </c>
       <c r="J7" t="n">
-        <v>11.5</v>
-      </c>
-      <c r="K7" t="inlineStr"/>
-      <c r="L7" t="inlineStr"/>
-      <c r="M7" t="inlineStr"/>
-      <c r="N7" t="inlineStr"/>
-      <c r="O7" t="inlineStr"/>
+        <v>-4</v>
+      </c>
+      <c r="K7" t="n">
+        <v>19</v>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>Utah State -19</t>
+        </is>
+      </c>
+      <c r="M7" t="n">
+        <v>1</v>
+      </c>
+      <c r="N7" t="n">
+        <v>1</v>
+      </c>
+      <c r="O7" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
@@ -793,46 +865,58 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Tulsa</t>
+          <t>Ohio State</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Navy</t>
+          <t>Ohio</t>
         </is>
       </c>
       <c r="D8" t="n">
         <v>4.7</v>
       </c>
       <c r="E8" t="n">
-        <v>6.9</v>
+        <v>7.600000000000001</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Navy -14.5</t>
+          <t>Ohio State -nan</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>Navy -13.5</t>
+          <t>Ohio State -28.5</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>Navy -6.6</t>
+          <t>Ohio State -36.1</t>
         </is>
       </c>
       <c r="I8" t="n">
-        <v>-6.6</v>
+        <v>36.1</v>
       </c>
       <c r="J8" t="n">
-        <v>-13.5</v>
-      </c>
-      <c r="K8" t="inlineStr"/>
-      <c r="L8" t="inlineStr"/>
-      <c r="M8" t="inlineStr"/>
-      <c r="N8" t="inlineStr"/>
-      <c r="O8" t="inlineStr"/>
+        <v>28.5</v>
+      </c>
+      <c r="K8" t="n">
+        <v>28</v>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>Ohio State -28</t>
+        </is>
+      </c>
+      <c r="M8" t="n">
+        <v>1</v>
+      </c>
+      <c r="N8" t="n">
+        <v>0</v>
+      </c>
+      <c r="O8" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
@@ -840,46 +924,58 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Temple</t>
+          <t>Tulsa</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Oklahoma</t>
+          <t>Navy</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>5.4</v>
+        <v>4.7</v>
       </c>
       <c r="E9" t="n">
-        <v>6.399999999999999</v>
+        <v>7.4</v>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Oklahoma -25.5</t>
+          <t>Tulsa -nan</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>Oklahoma -24.5</t>
+          <t>Navy -14</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>Oklahoma -18.1</t>
+          <t>Navy -6.6</t>
         </is>
       </c>
       <c r="I9" t="n">
-        <v>-18.1</v>
+        <v>-6.6</v>
       </c>
       <c r="J9" t="n">
-        <v>-24.5</v>
-      </c>
-      <c r="K9" t="inlineStr"/>
-      <c r="L9" t="inlineStr"/>
-      <c r="M9" t="inlineStr"/>
-      <c r="N9" t="inlineStr"/>
-      <c r="O9" t="inlineStr"/>
+        <v>-14</v>
+      </c>
+      <c r="K9" t="n">
+        <v>-19</v>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>Navy -19</t>
+        </is>
+      </c>
+      <c r="M9" t="n">
+        <v>1</v>
+      </c>
+      <c r="N9" t="n">
+        <v>0</v>
+      </c>
+      <c r="O9" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
@@ -887,46 +983,58 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Arizona State</t>
+          <t>Stanford</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Texas State</t>
+          <t>Boston College</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>8.300000000000001</v>
+        <v>6.3</v>
       </c>
       <c r="E10" t="n">
-        <v>5.9</v>
+        <v>7.3</v>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Arizona State -14.5</t>
+          <t>Boston College -12.5</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>Arizona State -15.5</t>
+          <t>Boston College -14</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>Arizona State -9.6</t>
+          <t>Boston College -6.7</t>
         </is>
       </c>
       <c r="I10" t="n">
-        <v>9.6</v>
+        <v>-6.7</v>
       </c>
       <c r="J10" t="n">
-        <v>15.5</v>
-      </c>
-      <c r="K10" t="inlineStr"/>
-      <c r="L10" t="inlineStr"/>
-      <c r="M10" t="inlineStr"/>
-      <c r="N10" t="inlineStr"/>
-      <c r="O10" t="inlineStr"/>
+        <v>-14</v>
+      </c>
+      <c r="K10" t="n">
+        <v>10</v>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>Stanford -10</t>
+        </is>
+      </c>
+      <c r="M10" t="n">
+        <v>1</v>
+      </c>
+      <c r="N10" t="n">
+        <v>1</v>
+      </c>
+      <c r="O10" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
@@ -934,46 +1042,58 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Northwestern</t>
+          <t>Auburn</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Oregon</t>
+          <t>South Alabama</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>5.8</v>
+        <v>6.2</v>
       </c>
       <c r="E11" t="n">
-        <v>5.399999999999999</v>
+        <v>6.600000000000001</v>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Oregon -27.5</t>
+          <t>Auburn -nan</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>Oregon -27.5</t>
+          <t>Auburn -26.5</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>Oregon -22.1</t>
+          <t>Auburn -19.9</t>
         </is>
       </c>
       <c r="I11" t="n">
-        <v>-22.1</v>
+        <v>19.9</v>
       </c>
       <c r="J11" t="n">
-        <v>-27.5</v>
-      </c>
-      <c r="K11" t="inlineStr"/>
-      <c r="L11" t="inlineStr"/>
-      <c r="M11" t="inlineStr"/>
-      <c r="N11" t="inlineStr"/>
-      <c r="O11" t="inlineStr"/>
+        <v>26.5</v>
+      </c>
+      <c r="K11" t="n">
+        <v>16</v>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>Auburn -16</t>
+        </is>
+      </c>
+      <c r="M11" t="n">
+        <v>1</v>
+      </c>
+      <c r="N11" t="n">
+        <v>1</v>
+      </c>
+      <c r="O11" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
@@ -981,46 +1101,58 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Purdue</t>
+          <t>Alabama</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>USC</t>
+          <t>Wisconsin</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>6.4</v>
+        <v>8.1</v>
       </c>
       <c r="E12" t="n">
-        <v>5.300000000000001</v>
+        <v>6.399999999999999</v>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>USC -21.5</t>
+          <t>Alabama -nan</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>USC -21.5</t>
+          <t>Alabama -17.5</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>USC -16.2</t>
+          <t>Alabama -23.9</t>
         </is>
       </c>
       <c r="I12" t="n">
-        <v>-16.2</v>
+        <v>23.9</v>
       </c>
       <c r="J12" t="n">
-        <v>-21.5</v>
-      </c>
-      <c r="K12" t="inlineStr"/>
-      <c r="L12" t="inlineStr"/>
-      <c r="M12" t="inlineStr"/>
-      <c r="N12" t="inlineStr"/>
-      <c r="O12" t="inlineStr"/>
+        <v>17.5</v>
+      </c>
+      <c r="K12" t="n">
+        <v>24</v>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>Alabama -24</t>
+        </is>
+      </c>
+      <c r="M12" t="n">
+        <v>1</v>
+      </c>
+      <c r="N12" t="n">
+        <v>1</v>
+      </c>
+      <c r="O12" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
@@ -1028,46 +1160,58 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Nevada</t>
+          <t>UAB</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Middle Tennessee</t>
+          <t>Akron</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>5.6</v>
+        <v>3</v>
       </c>
       <c r="E13" t="n">
-        <v>5.1</v>
+        <v>6.399999999999999</v>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>Nevada -9.5</t>
+          <t>UAB -nan</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>Nevada -9.5</t>
+          <t>UAB -12.5</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>Nevada -4.4</t>
+          <t>UAB -18.9</t>
         </is>
       </c>
       <c r="I13" t="n">
-        <v>4.4</v>
+        <v>18.9</v>
       </c>
       <c r="J13" t="n">
-        <v>9.5</v>
-      </c>
-      <c r="K13" t="inlineStr"/>
-      <c r="L13" t="inlineStr"/>
-      <c r="M13" t="inlineStr"/>
-      <c r="N13" t="inlineStr"/>
-      <c r="O13" t="inlineStr"/>
+        <v>12.5</v>
+      </c>
+      <c r="K13" t="n">
+        <v>3</v>
+      </c>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>UAB -3</t>
+        </is>
+      </c>
+      <c r="M13" t="n">
+        <v>1</v>
+      </c>
+      <c r="N13" t="n">
+        <v>0</v>
+      </c>
+      <c r="O13" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
@@ -1075,46 +1219,58 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Arkansas State</t>
+          <t>Arizona</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Iowa State</t>
+          <t>Kansas State</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>3.7</v>
+        <v>8.9</v>
       </c>
       <c r="E14" t="n">
-        <v>4.9</v>
+        <v>5.9</v>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>Iowa State -21.5</t>
+          <t>Arizona -nan</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>Iowa State -20.5</t>
+          <t>Kansas State -1.5</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>Iowa State -15.6</t>
+          <t>Arizona -4.4</t>
         </is>
       </c>
       <c r="I14" t="n">
-        <v>-15.6</v>
+        <v>4.4</v>
       </c>
       <c r="J14" t="n">
-        <v>-20.5</v>
-      </c>
-      <c r="K14" t="inlineStr"/>
-      <c r="L14" t="inlineStr"/>
-      <c r="M14" t="inlineStr"/>
-      <c r="N14" t="inlineStr"/>
-      <c r="O14" t="inlineStr"/>
+        <v>-1.5</v>
+      </c>
+      <c r="K14" t="n">
+        <v>6</v>
+      </c>
+      <c r="L14" t="inlineStr">
+        <is>
+          <t>Arizona -6</t>
+        </is>
+      </c>
+      <c r="M14" t="n">
+        <v>1</v>
+      </c>
+      <c r="N14" t="n">
+        <v>1</v>
+      </c>
+      <c r="O14" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
@@ -1122,46 +1278,58 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Auburn</t>
+          <t>Virginia Tech</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>South Alabama</t>
+          <t>Old Dominion</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>6.2</v>
+        <v>6.9</v>
       </c>
       <c r="E15" t="n">
-        <v>4.699999999999999</v>
+        <v>5.4</v>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>Auburn -25.5</t>
+          <t>Virginia Tech -nan</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>Auburn -24.5</t>
+          <t>Virginia Tech -5.5</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>Auburn -19.8</t>
+          <t>Virginia Tech -10.9</t>
         </is>
       </c>
       <c r="I15" t="n">
-        <v>19.8</v>
+        <v>10.9</v>
       </c>
       <c r="J15" t="n">
-        <v>24.5</v>
-      </c>
-      <c r="K15" t="inlineStr"/>
-      <c r="L15" t="inlineStr"/>
-      <c r="M15" t="inlineStr"/>
-      <c r="N15" t="inlineStr"/>
-      <c r="O15" t="inlineStr"/>
+        <v>5.5</v>
+      </c>
+      <c r="K15" t="n">
+        <v>-19</v>
+      </c>
+      <c r="L15" t="inlineStr">
+        <is>
+          <t>Old Dominion -19</t>
+        </is>
+      </c>
+      <c r="M15" t="n">
+        <v>1</v>
+      </c>
+      <c r="N15" t="n">
+        <v>0</v>
+      </c>
+      <c r="O15" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
@@ -1169,46 +1337,58 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Texas</t>
+          <t>Arkansas State</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>UTEP</t>
+          <t>Iowa State</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>3.4</v>
+        <v>3.7</v>
       </c>
       <c r="E16" t="n">
-        <v>4</v>
+        <v>5.4</v>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>Texas -36.5</t>
+          <t>Arkansas State -nan</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>Texas -41.5</t>
+          <t>Iowa State -21</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>Texas -37.5</t>
+          <t>Iowa State -15.6</t>
         </is>
       </c>
       <c r="I16" t="n">
-        <v>37.5</v>
+        <v>-15.6</v>
       </c>
       <c r="J16" t="n">
-        <v>41.5</v>
-      </c>
-      <c r="K16" t="inlineStr"/>
-      <c r="L16" t="inlineStr"/>
-      <c r="M16" t="inlineStr"/>
-      <c r="N16" t="inlineStr"/>
-      <c r="O16" t="inlineStr"/>
+        <v>-21</v>
+      </c>
+      <c r="K16" t="n">
+        <v>-8</v>
+      </c>
+      <c r="L16" t="inlineStr">
+        <is>
+          <t>Iowa State -8</t>
+        </is>
+      </c>
+      <c r="M16" t="n">
+        <v>1</v>
+      </c>
+      <c r="N16" t="n">
+        <v>1</v>
+      </c>
+      <c r="O16" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
@@ -1216,46 +1396,58 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Tulane</t>
+          <t>Temple</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Duke</t>
+          <t>Oklahoma</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>8.300000000000001</v>
+        <v>5.4</v>
       </c>
       <c r="E17" t="n">
-        <v>3.9</v>
+        <v>5.300000000000001</v>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>Tulane -2.5</t>
+          <t>Temple -nan</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>Tulane -2.5</t>
+          <t>Oklahoma -23.5</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>Tulane -6.4</t>
+          <t>Oklahoma -18.2</t>
         </is>
       </c>
       <c r="I17" t="n">
-        <v>6.4</v>
+        <v>-18.2</v>
       </c>
       <c r="J17" t="n">
-        <v>2.5</v>
-      </c>
-      <c r="K17" t="inlineStr"/>
-      <c r="L17" t="inlineStr"/>
-      <c r="M17" t="inlineStr"/>
-      <c r="N17" t="inlineStr"/>
-      <c r="O17" t="inlineStr"/>
+        <v>-23.5</v>
+      </c>
+      <c r="K17" t="n">
+        <v>-39</v>
+      </c>
+      <c r="L17" t="inlineStr">
+        <is>
+          <t>Oklahoma -39</t>
+        </is>
+      </c>
+      <c r="M17" t="n">
+        <v>1</v>
+      </c>
+      <c r="N17" t="n">
+        <v>0</v>
+      </c>
+      <c r="O17" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
@@ -1263,46 +1455,58 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Iowa</t>
+          <t>Nevada</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Massachusetts</t>
+          <t>Middle Tennessee</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>2.3</v>
+        <v>5.6</v>
       </c>
       <c r="E18" t="n">
-        <v>3.899999999999999</v>
+        <v>5.1</v>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>Iowa -33.5</t>
+          <t>Nevada -nan</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>Iowa -34.5</t>
+          <t>Nevada -9.5</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>Iowa -30.6</t>
+          <t>Nevada -4.4</t>
         </is>
       </c>
       <c r="I18" t="n">
-        <v>30.6</v>
+        <v>4.4</v>
       </c>
       <c r="J18" t="n">
-        <v>34.5</v>
-      </c>
-      <c r="K18" t="inlineStr"/>
-      <c r="L18" t="inlineStr"/>
-      <c r="M18" t="inlineStr"/>
-      <c r="N18" t="inlineStr"/>
-      <c r="O18" t="inlineStr"/>
+        <v>9.5</v>
+      </c>
+      <c r="K18" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L18" t="inlineStr">
+        <is>
+          <t>Middle Tennessee -1</t>
+        </is>
+      </c>
+      <c r="M18" t="n">
+        <v>1</v>
+      </c>
+      <c r="N18" t="n">
+        <v>1</v>
+      </c>
+      <c r="O18" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
@@ -1310,46 +1514,58 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Houston</t>
+          <t>South Carolina</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Colorado</t>
+          <t>Vanderbilt</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>8.199999999999999</v>
+        <v>9.199999999999999</v>
       </c>
       <c r="E19" t="n">
-        <v>3.8</v>
+        <v>5</v>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>Houston -3.5</t>
+          <t>South Carolina -nan</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>Houston -5.5</t>
+          <t>South Carolina -3</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>Houston -1.7</t>
+          <t>South Carolina -8.0</t>
         </is>
       </c>
       <c r="I19" t="n">
-        <v>1.7</v>
+        <v>8</v>
       </c>
       <c r="J19" t="n">
-        <v>5.5</v>
-      </c>
-      <c r="K19" t="inlineStr"/>
-      <c r="L19" t="inlineStr"/>
-      <c r="M19" t="inlineStr"/>
-      <c r="N19" t="inlineStr"/>
-      <c r="O19" t="inlineStr"/>
+        <v>3</v>
+      </c>
+      <c r="K19" t="n">
+        <v>-24</v>
+      </c>
+      <c r="L19" t="inlineStr">
+        <is>
+          <t>Vanderbilt -24</t>
+        </is>
+      </c>
+      <c r="M19" t="n">
+        <v>1</v>
+      </c>
+      <c r="N19" t="n">
+        <v>0</v>
+      </c>
+      <c r="O19" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
@@ -1357,46 +1573,58 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Stanford</t>
+          <t>Tulane</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Boston College</t>
+          <t>Duke</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>6.3</v>
+        <v>8.300000000000001</v>
       </c>
       <c r="E20" t="n">
-        <v>3.8</v>
+        <v>4.9</v>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>Boston College -10.5</t>
+          <t>Tulane -nan</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>Boston College -10.5</t>
+          <t>Tulane -1.5</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>Boston College -6.7</t>
+          <t>Tulane -6.4</t>
         </is>
       </c>
       <c r="I20" t="n">
-        <v>-6.7</v>
+        <v>6.4</v>
       </c>
       <c r="J20" t="n">
-        <v>-10.5</v>
-      </c>
-      <c r="K20" t="inlineStr"/>
-      <c r="L20" t="inlineStr"/>
-      <c r="M20" t="inlineStr"/>
-      <c r="N20" t="inlineStr"/>
-      <c r="O20" t="inlineStr"/>
+        <v>1.5</v>
+      </c>
+      <c r="K20" t="n">
+        <v>7</v>
+      </c>
+      <c r="L20" t="inlineStr">
+        <is>
+          <t>Tulane -7</t>
+        </is>
+      </c>
+      <c r="M20" t="n">
+        <v>1</v>
+      </c>
+      <c r="N20" t="n">
+        <v>1</v>
+      </c>
+      <c r="O20" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
@@ -1404,46 +1632,58 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Ohio State</t>
+          <t>Iowa</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Ohio</t>
+          <t>Massachusetts</t>
         </is>
       </c>
       <c r="D21" t="n">
-        <v>4.7</v>
+        <v>2.3</v>
       </c>
       <c r="E21" t="n">
-        <v>3.600000000000001</v>
+        <v>4.800000000000001</v>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>Ohio State -25.5</t>
+          <t>Iowa -35.5</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>Ohio State -32.5</t>
+          <t>Iowa -35.5</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>Ohio State -36.1</t>
+          <t>Iowa -30.7</t>
         </is>
       </c>
       <c r="I21" t="n">
-        <v>36.1</v>
+        <v>30.7</v>
       </c>
       <c r="J21" t="n">
-        <v>32.5</v>
-      </c>
-      <c r="K21" t="inlineStr"/>
-      <c r="L21" t="inlineStr"/>
-      <c r="M21" t="inlineStr"/>
-      <c r="N21" t="inlineStr"/>
-      <c r="O21" t="inlineStr"/>
+        <v>35.5</v>
+      </c>
+      <c r="K21" t="n">
+        <v>40</v>
+      </c>
+      <c r="L21" t="inlineStr">
+        <is>
+          <t>Iowa -40</t>
+        </is>
+      </c>
+      <c r="M21" t="n">
+        <v>0</v>
+      </c>
+      <c r="N21" t="n">
+        <v>0</v>
+      </c>
+      <c r="O21" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
@@ -1451,46 +1691,58 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Virginia Tech</t>
+          <t>Kentucky</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Old Dominion</t>
+          <t>Eastern Michigan</t>
         </is>
       </c>
       <c r="D22" t="n">
-        <v>6.9</v>
+        <v>3.8</v>
       </c>
       <c r="E22" t="n">
-        <v>3.6</v>
+        <v>4.399999999999999</v>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>Virginia Tech -6.5</t>
+          <t>Kentucky -nan</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>Virginia Tech -7.5</t>
+          <t>Kentucky -26.5</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>Virginia Tech -11.1</t>
+          <t>Kentucky -22.1</t>
         </is>
       </c>
       <c r="I22" t="n">
-        <v>11.1</v>
+        <v>22.1</v>
       </c>
       <c r="J22" t="n">
-        <v>7.5</v>
-      </c>
-      <c r="K22" t="inlineStr"/>
-      <c r="L22" t="inlineStr"/>
-      <c r="M22" t="inlineStr"/>
-      <c r="N22" t="inlineStr"/>
-      <c r="O22" t="inlineStr"/>
+        <v>26.5</v>
+      </c>
+      <c r="K22" t="n">
+        <v>25</v>
+      </c>
+      <c r="L22" t="inlineStr">
+        <is>
+          <t>Kentucky -25</t>
+        </is>
+      </c>
+      <c r="M22" t="n">
+        <v>1</v>
+      </c>
+      <c r="N22" t="n">
+        <v>1</v>
+      </c>
+      <c r="O22" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
@@ -1498,46 +1750,58 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Alabama</t>
+          <t>Purdue</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Wisconsin</t>
+          <t>USC</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>8.1</v>
+        <v>6.4</v>
       </c>
       <c r="E23" t="n">
-        <v>3.300000000000001</v>
+        <v>4.300000000000001</v>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>Alabama -22.5</t>
+          <t>Purdue -nan</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>Alabama -20.5</t>
+          <t>USC -20.5</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>Alabama -23.8</t>
+          <t>USC -16.2</t>
         </is>
       </c>
       <c r="I23" t="n">
-        <v>23.8</v>
+        <v>-16.2</v>
       </c>
       <c r="J23" t="n">
-        <v>20.5</v>
-      </c>
-      <c r="K23" t="inlineStr"/>
-      <c r="L23" t="inlineStr"/>
-      <c r="M23" t="inlineStr"/>
-      <c r="N23" t="inlineStr"/>
-      <c r="O23" t="inlineStr"/>
+        <v>-20.5</v>
+      </c>
+      <c r="K23" t="n">
+        <v>-16</v>
+      </c>
+      <c r="L23" t="inlineStr">
+        <is>
+          <t>USC -16</t>
+        </is>
+      </c>
+      <c r="M23" t="n">
+        <v>1</v>
+      </c>
+      <c r="N23" t="n">
+        <v>1</v>
+      </c>
+      <c r="O23" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
@@ -1545,46 +1809,58 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Tennessee</t>
+          <t>Ole Miss</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Georgia</t>
+          <t>Arkansas</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>9.6</v>
+        <v>9.4</v>
       </c>
       <c r="E24" t="n">
-        <v>3.2</v>
+        <v>4.3</v>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>Georgia -7.5</t>
+          <t>Ole Miss -nan</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>Georgia -7.5</t>
+          <t>Ole Miss -3.5</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>Georgia -4.3</t>
+          <t>Ole Miss -7.8</t>
         </is>
       </c>
       <c r="I24" t="n">
-        <v>-4.3</v>
+        <v>7.8</v>
       </c>
       <c r="J24" t="n">
-        <v>-7.5</v>
-      </c>
-      <c r="K24" t="inlineStr"/>
-      <c r="L24" t="inlineStr"/>
-      <c r="M24" t="inlineStr"/>
-      <c r="N24" t="inlineStr"/>
-      <c r="O24" t="inlineStr"/>
+        <v>3.5</v>
+      </c>
+      <c r="K24" t="n">
+        <v>6</v>
+      </c>
+      <c r="L24" t="inlineStr">
+        <is>
+          <t>Ole Miss -6</t>
+        </is>
+      </c>
+      <c r="M24" t="n">
+        <v>1</v>
+      </c>
+      <c r="N24" t="n">
+        <v>1</v>
+      </c>
+      <c r="O24" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
@@ -1592,46 +1868,58 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Wake Forest</t>
+          <t>North Texas</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>NC State</t>
+          <t>Washington State</t>
         </is>
       </c>
       <c r="D25" t="n">
-        <v>7.1</v>
+        <v>7.7</v>
       </c>
       <c r="E25" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>North Texas -nan</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>North Texas -6.5</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>North Texas -3.0</t>
+        </is>
+      </c>
+      <c r="I25" t="n">
         <v>3</v>
       </c>
-      <c r="F25" t="inlineStr">
-        <is>
-          <t>NC State -7.5</t>
-        </is>
-      </c>
-      <c r="G25" t="inlineStr">
-        <is>
-          <t>NC State -7.5</t>
-        </is>
-      </c>
-      <c r="H25" t="inlineStr">
-        <is>
-          <t>NC State -4.5</t>
-        </is>
-      </c>
-      <c r="I25" t="n">
-        <v>-4.5</v>
-      </c>
       <c r="J25" t="n">
-        <v>-7.5</v>
-      </c>
-      <c r="K25" t="inlineStr"/>
-      <c r="L25" t="inlineStr"/>
-      <c r="M25" t="inlineStr"/>
-      <c r="N25" t="inlineStr"/>
-      <c r="O25" t="inlineStr"/>
+        <v>6.5</v>
+      </c>
+      <c r="K25" t="n">
+        <v>49</v>
+      </c>
+      <c r="L25" t="inlineStr">
+        <is>
+          <t>North Texas -49</t>
+        </is>
+      </c>
+      <c r="M25" t="n">
+        <v>1</v>
+      </c>
+      <c r="N25" t="n">
+        <v>0</v>
+      </c>
+      <c r="O25" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
@@ -1639,46 +1927,58 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Arizona</t>
+          <t>Georgia Tech</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Kansas State</t>
+          <t>Clemson</t>
         </is>
       </c>
       <c r="D26" t="n">
-        <v>8.9</v>
+        <v>8.800000000000001</v>
       </c>
       <c r="E26" t="n">
-        <v>2.9</v>
+        <v>3.4</v>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>Kansas State -1.5</t>
+          <t>Clemson -8.5</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>Arizona -1.5</t>
+          <t>Clemson -3</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>Arizona -4.4</t>
+          <t>Clemson -6.4</t>
         </is>
       </c>
       <c r="I26" t="n">
-        <v>4.4</v>
+        <v>-6.4</v>
       </c>
       <c r="J26" t="n">
-        <v>1.5</v>
-      </c>
-      <c r="K26" t="inlineStr"/>
-      <c r="L26" t="inlineStr"/>
-      <c r="M26" t="inlineStr"/>
-      <c r="N26" t="inlineStr"/>
-      <c r="O26" t="inlineStr"/>
+        <v>-3</v>
+      </c>
+      <c r="K26" t="n">
+        <v>3</v>
+      </c>
+      <c r="L26" t="inlineStr">
+        <is>
+          <t>Georgia Tech -3</t>
+        </is>
+      </c>
+      <c r="M26" t="n">
+        <v>1</v>
+      </c>
+      <c r="N26" t="n">
+        <v>0</v>
+      </c>
+      <c r="O26" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
@@ -1686,46 +1986,58 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>UCLA</t>
+          <t>West Virginia</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>New Mexico</t>
+          <t>Pittsburgh</t>
         </is>
       </c>
       <c r="D27" t="n">
-        <v>3.3</v>
+        <v>7.9</v>
       </c>
       <c r="E27" t="n">
-        <v>2.800000000000001</v>
+        <v>3.4</v>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>UCLA -14.5</t>
+          <t>Pittsburgh -2.5</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>UCLA -15.5</t>
+          <t>Pittsburgh -7</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>UCLA -18.3</t>
+          <t>Pittsburgh -3.6</t>
         </is>
       </c>
       <c r="I27" t="n">
-        <v>18.3</v>
+        <v>-3.6</v>
       </c>
       <c r="J27" t="n">
-        <v>15.5</v>
-      </c>
-      <c r="K27" t="inlineStr"/>
-      <c r="L27" t="inlineStr"/>
-      <c r="M27" t="inlineStr"/>
-      <c r="N27" t="inlineStr"/>
-      <c r="O27" t="inlineStr"/>
+        <v>-7</v>
+      </c>
+      <c r="K27" t="n">
+        <v>7</v>
+      </c>
+      <c r="L27" t="inlineStr">
+        <is>
+          <t>West Virginia -7</t>
+        </is>
+      </c>
+      <c r="M27" t="n">
+        <v>0</v>
+      </c>
+      <c r="N27" t="n">
+        <v>1</v>
+      </c>
+      <c r="O27" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
@@ -1733,46 +2045,58 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Delaware</t>
+          <t>Northwestern</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>UConn</t>
+          <t>Oregon</t>
         </is>
       </c>
       <c r="D28" t="n">
-        <v>3.4</v>
+        <v>5.8</v>
       </c>
       <c r="E28" t="n">
-        <v>2.8</v>
+        <v>3.399999999999999</v>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>UConn -10.5</t>
+          <t>Northwestern -nan</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>UConn -10.5</t>
+          <t>Oregon -25.5</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>UConn -7.7</t>
+          <t>Oregon -22.1</t>
         </is>
       </c>
       <c r="I28" t="n">
-        <v>-7.7</v>
+        <v>-22.1</v>
       </c>
       <c r="J28" t="n">
-        <v>-10.5</v>
-      </c>
-      <c r="K28" t="inlineStr"/>
-      <c r="L28" t="inlineStr"/>
-      <c r="M28" t="inlineStr"/>
-      <c r="N28" t="inlineStr"/>
-      <c r="O28" t="inlineStr"/>
+        <v>-25.5</v>
+      </c>
+      <c r="K28" t="n">
+        <v>-20</v>
+      </c>
+      <c r="L28" t="inlineStr">
+        <is>
+          <t>Oregon -20</t>
+        </is>
+      </c>
+      <c r="M28" t="n">
+        <v>1</v>
+      </c>
+      <c r="N28" t="n">
+        <v>1</v>
+      </c>
+      <c r="O28" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
@@ -1780,46 +2104,58 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Southern Miss</t>
+          <t>Wake Forest</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>App State</t>
+          <t>NC State</t>
         </is>
       </c>
       <c r="D29" t="n">
-        <v>5.6</v>
+        <v>7.1</v>
       </c>
       <c r="E29" t="n">
-        <v>2.7</v>
+        <v>2.9</v>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>Southern Miss -2.5</t>
+          <t>Wake Forest -nan</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>Southern Miss -1.5</t>
+          <t>NC State -7.5</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>App State -1.2</t>
+          <t>NC State -4.6</t>
         </is>
       </c>
       <c r="I29" t="n">
-        <v>-1.2</v>
+        <v>-4.6</v>
       </c>
       <c r="J29" t="n">
-        <v>1.5</v>
-      </c>
-      <c r="K29" t="inlineStr"/>
-      <c r="L29" t="inlineStr"/>
-      <c r="M29" t="inlineStr"/>
-      <c r="N29" t="inlineStr"/>
-      <c r="O29" t="inlineStr"/>
+        <v>-7.5</v>
+      </c>
+      <c r="K29" t="n">
+        <v>-10</v>
+      </c>
+      <c r="L29" t="inlineStr">
+        <is>
+          <t>NC State -10</t>
+        </is>
+      </c>
+      <c r="M29" t="n">
+        <v>1</v>
+      </c>
+      <c r="N29" t="n">
+        <v>0</v>
+      </c>
+      <c r="O29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
@@ -1827,46 +2163,58 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>South Carolina</t>
+          <t>UCLA</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Vanderbilt</t>
+          <t>New Mexico</t>
         </is>
       </c>
       <c r="D30" t="n">
-        <v>9.199999999999999</v>
+        <v>3.3</v>
       </c>
       <c r="E30" t="n">
-        <v>2.699999999999999</v>
+        <v>2.5</v>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>South Carolina -5.5</t>
+          <t>UCLA -nan</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>South Carolina -5.5</t>
+          <t>UCLA -15.5</t>
         </is>
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>South Carolina -8.2</t>
+          <t>UCLA -18.0</t>
         </is>
       </c>
       <c r="I30" t="n">
-        <v>8.199999999999999</v>
+        <v>18</v>
       </c>
       <c r="J30" t="n">
-        <v>5.5</v>
-      </c>
-      <c r="K30" t="inlineStr"/>
-      <c r="L30" t="inlineStr"/>
-      <c r="M30" t="inlineStr"/>
-      <c r="N30" t="inlineStr"/>
-      <c r="O30" t="inlineStr"/>
+        <v>15.5</v>
+      </c>
+      <c r="K30" t="n">
+        <v>-25</v>
+      </c>
+      <c r="L30" t="inlineStr">
+        <is>
+          <t>New Mexico -25</t>
+        </is>
+      </c>
+      <c r="M30" t="n">
+        <v>1</v>
+      </c>
+      <c r="N30" t="n">
+        <v>0</v>
+      </c>
+      <c r="O30" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="n">
@@ -1874,46 +2222,58 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Kentucky</t>
+          <t>Houston</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Eastern Michigan</t>
+          <t>Colorado</t>
         </is>
       </c>
       <c r="D31" t="n">
-        <v>3.8</v>
+        <v>8.199999999999999</v>
       </c>
       <c r="E31" t="n">
-        <v>2.399999999999999</v>
+        <v>2.2</v>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>Kentucky -25.5</t>
+          <t>Houston -nan</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>Kentucky -24.5</t>
+          <t>Houston -4</t>
         </is>
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>Kentucky -22.1</t>
+          <t>Houston -1.8</t>
         </is>
       </c>
       <c r="I31" t="n">
-        <v>22.1</v>
+        <v>1.8</v>
       </c>
       <c r="J31" t="n">
-        <v>24.5</v>
-      </c>
-      <c r="K31" t="inlineStr"/>
-      <c r="L31" t="inlineStr"/>
-      <c r="M31" t="inlineStr"/>
-      <c r="N31" t="inlineStr"/>
-      <c r="O31" t="inlineStr"/>
+        <v>4</v>
+      </c>
+      <c r="K31" t="n">
+        <v>16</v>
+      </c>
+      <c r="L31" t="inlineStr">
+        <is>
+          <t>Houston -16</t>
+        </is>
+      </c>
+      <c r="M31" t="n">
+        <v>1</v>
+      </c>
+      <c r="N31" t="n">
+        <v>0</v>
+      </c>
+      <c r="O31" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
@@ -1921,46 +2281,58 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Georgia Tech</t>
+          <t>Texas</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Clemson</t>
+          <t>UTEP</t>
         </is>
       </c>
       <c r="D32" t="n">
-        <v>8.800000000000001</v>
+        <v>3.4</v>
       </c>
       <c r="E32" t="n">
-        <v>2.1</v>
+        <v>2</v>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>Clemson -8.5</t>
+          <t>Texas -nan</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>Clemson -8.5</t>
+          <t>Texas -39.5</t>
         </is>
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>Clemson -6.4</t>
+          <t>Texas -37.5</t>
         </is>
       </c>
       <c r="I32" t="n">
-        <v>-6.4</v>
+        <v>37.5</v>
       </c>
       <c r="J32" t="n">
-        <v>-8.5</v>
-      </c>
-      <c r="K32" t="inlineStr"/>
-      <c r="L32" t="inlineStr"/>
-      <c r="M32" t="inlineStr"/>
-      <c r="N32" t="inlineStr"/>
-      <c r="O32" t="inlineStr"/>
+        <v>39.5</v>
+      </c>
+      <c r="K32" t="n">
+        <v>17</v>
+      </c>
+      <c r="L32" t="inlineStr">
+        <is>
+          <t>Texas -17</t>
+        </is>
+      </c>
+      <c r="M32" t="n">
+        <v>1</v>
+      </c>
+      <c r="N32" t="n">
+        <v>1</v>
+      </c>
+      <c r="O32" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
@@ -1968,46 +2340,58 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>North Texas</t>
+          <t>Notre Dame</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Washington State</t>
+          <t>Texas A&amp;M</t>
         </is>
       </c>
       <c r="D33" t="n">
-        <v>7.7</v>
+        <v>9.800000000000001</v>
       </c>
       <c r="E33" t="n">
-        <v>1.9</v>
+        <v>2</v>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>North Texas -5.5</t>
+          <t>Notre Dame -7.0</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>North Texas -4.5</t>
+          <t>Notre Dame -6.5</t>
         </is>
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>North Texas -2.6</t>
+          <t>Notre Dame -8.5</t>
         </is>
       </c>
       <c r="I33" t="n">
-        <v>2.6</v>
+        <v>8.5</v>
       </c>
       <c r="J33" t="n">
-        <v>4.5</v>
-      </c>
-      <c r="K33" t="inlineStr"/>
-      <c r="L33" t="inlineStr"/>
-      <c r="M33" t="inlineStr"/>
-      <c r="N33" t="inlineStr"/>
-      <c r="O33" t="inlineStr"/>
+        <v>6.5</v>
+      </c>
+      <c r="K33" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L33" t="inlineStr">
+        <is>
+          <t>Texas A&amp;M -1</t>
+        </is>
+      </c>
+      <c r="M33" t="n">
+        <v>0</v>
+      </c>
+      <c r="N33" t="n">
+        <v>0</v>
+      </c>
+      <c r="O33" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="n">
@@ -2015,46 +2399,58 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Ole Miss</t>
+          <t>Southern Miss</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Arkansas</t>
+          <t>App State</t>
         </is>
       </c>
       <c r="D34" t="n">
-        <v>9.4</v>
+        <v>5.6</v>
       </c>
       <c r="E34" t="n">
-        <v>1.7</v>
+        <v>1.9</v>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>Ole Miss -8.5</t>
+          <t>Southern Miss -nan</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>Ole Miss -9.5</t>
+          <t>App State -3</t>
         </is>
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>Ole Miss -7.8</t>
+          <t>App State -1.1</t>
         </is>
       </c>
       <c r="I34" t="n">
-        <v>7.8</v>
+        <v>-1.1</v>
       </c>
       <c r="J34" t="n">
-        <v>9.5</v>
-      </c>
-      <c r="K34" t="inlineStr"/>
-      <c r="L34" t="inlineStr"/>
-      <c r="M34" t="inlineStr"/>
-      <c r="N34" t="inlineStr"/>
-      <c r="O34" t="inlineStr"/>
+        <v>-3</v>
+      </c>
+      <c r="K34" t="n">
+        <v>16</v>
+      </c>
+      <c r="L34" t="inlineStr">
+        <is>
+          <t>Southern Miss -16</t>
+        </is>
+      </c>
+      <c r="M34" t="n">
+        <v>1</v>
+      </c>
+      <c r="N34" t="n">
+        <v>1</v>
+      </c>
+      <c r="O34" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="n">
@@ -2062,46 +2458,58 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Notre Dame</t>
+          <t>LSU</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Texas A&amp;M</t>
+          <t>Florida</t>
         </is>
       </c>
       <c r="D35" t="n">
         <v>9.800000000000001</v>
       </c>
       <c r="E35" t="n">
-        <v>1.6</v>
+        <v>1.8</v>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>Notre Dame -7.0</t>
+          <t>LSU -5.5</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>Notre Dame -7</t>
+          <t>LSU -4.5</t>
         </is>
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>Notre Dame -8.6</t>
+          <t>LSU -6.3</t>
         </is>
       </c>
       <c r="I35" t="n">
-        <v>8.6</v>
+        <v>6.3</v>
       </c>
       <c r="J35" t="n">
-        <v>7</v>
-      </c>
-      <c r="K35" t="inlineStr"/>
-      <c r="L35" t="inlineStr"/>
-      <c r="M35" t="inlineStr"/>
-      <c r="N35" t="inlineStr"/>
-      <c r="O35" t="inlineStr"/>
+        <v>4.5</v>
+      </c>
+      <c r="K35" t="n">
+        <v>10</v>
+      </c>
+      <c r="L35" t="inlineStr">
+        <is>
+          <t>LSU -10</t>
+        </is>
+      </c>
+      <c r="M35" t="n">
+        <v>1</v>
+      </c>
+      <c r="N35" t="n">
+        <v>1</v>
+      </c>
+      <c r="O35" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="n">
@@ -2121,11 +2529,11 @@
         <v>6.7</v>
       </c>
       <c r="E36" t="n">
-        <v>1.6</v>
+        <v>1.7</v>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>Florida International -4.5</t>
+          <t>Florida International -nan</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
@@ -2135,20 +2543,32 @@
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>Florida International -4.1</t>
+          <t>Florida International -4.2</t>
         </is>
       </c>
       <c r="I36" t="n">
-        <v>4.1</v>
+        <v>4.2</v>
       </c>
       <c r="J36" t="n">
         <v>2.5</v>
       </c>
-      <c r="K36" t="inlineStr"/>
-      <c r="L36" t="inlineStr"/>
-      <c r="M36" t="inlineStr"/>
-      <c r="N36" t="inlineStr"/>
-      <c r="O36" t="inlineStr"/>
+      <c r="K36" t="n">
+        <v>10</v>
+      </c>
+      <c r="L36" t="inlineStr">
+        <is>
+          <t>Florida International -10</t>
+        </is>
+      </c>
+      <c r="M36" t="n">
+        <v>1</v>
+      </c>
+      <c r="N36" t="n">
+        <v>1</v>
+      </c>
+      <c r="O36" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="n">
@@ -2156,46 +2576,58 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>West Virginia</t>
+          <t>California</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Pittsburgh</t>
+          <t>Minnesota</t>
         </is>
       </c>
       <c r="D37" t="n">
-        <v>7.9</v>
+        <v>8</v>
       </c>
       <c r="E37" t="n">
-        <v>1.1</v>
+        <v>1.2</v>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>Pittsburgh -2.5</t>
+          <t>California -nan</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>Pittsburgh -2.5</t>
+          <t>Minnesota -3</t>
         </is>
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>Pittsburgh -3.6</t>
+          <t>Minnesota -1.8</t>
         </is>
       </c>
       <c r="I37" t="n">
-        <v>-3.6</v>
+        <v>-1.8</v>
       </c>
       <c r="J37" t="n">
-        <v>-2.5</v>
-      </c>
-      <c r="K37" t="inlineStr"/>
-      <c r="L37" t="inlineStr"/>
-      <c r="M37" t="inlineStr"/>
-      <c r="N37" t="inlineStr"/>
-      <c r="O37" t="inlineStr"/>
+        <v>-3</v>
+      </c>
+      <c r="K37" t="n">
+        <v>13</v>
+      </c>
+      <c r="L37" t="inlineStr">
+        <is>
+          <t>California -13</t>
+        </is>
+      </c>
+      <c r="M37" t="n">
+        <v>1</v>
+      </c>
+      <c r="N37" t="n">
+        <v>1</v>
+      </c>
+      <c r="O37" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="n">
@@ -2203,46 +2635,58 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Illinois</t>
+          <t>Texas Tech</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Western Michigan</t>
+          <t>Oregon State</t>
         </is>
       </c>
       <c r="D38" t="n">
-        <v>3.3</v>
+        <v>5.4</v>
       </c>
       <c r="E38" t="n">
-        <v>1</v>
+        <v>1.199999999999999</v>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>Illinois -28.5</t>
+          <t>Texas Tech -nan</t>
         </is>
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>Illinois -27.5</t>
+          <t>Texas Tech -24.5</t>
         </is>
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>Illinois -26.5</t>
+          <t>Texas Tech -23.3</t>
         </is>
       </c>
       <c r="I38" t="n">
-        <v>26.5</v>
+        <v>23.3</v>
       </c>
       <c r="J38" t="n">
-        <v>27.5</v>
-      </c>
-      <c r="K38" t="inlineStr"/>
-      <c r="L38" t="inlineStr"/>
-      <c r="M38" t="inlineStr"/>
-      <c r="N38" t="inlineStr"/>
-      <c r="O38" t="inlineStr"/>
+        <v>24.5</v>
+      </c>
+      <c r="K38" t="n">
+        <v>38</v>
+      </c>
+      <c r="L38" t="inlineStr">
+        <is>
+          <t>Texas Tech -38</t>
+        </is>
+      </c>
+      <c r="M38" t="n">
+        <v>1</v>
+      </c>
+      <c r="N38" t="n">
+        <v>0</v>
+      </c>
+      <c r="O38" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="n">
@@ -2250,46 +2694,58 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Georgia Southern</t>
+          <t>Missouri State</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Jacksonville State</t>
+          <t>SMU</t>
         </is>
       </c>
       <c r="D39" t="n">
-        <v>6.6</v>
+        <v>2</v>
       </c>
       <c r="E39" t="n">
-        <v>1</v>
+        <v>1.199999999999999</v>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>Georgia Southern -2.5</t>
+          <t>Missouri State -nan</t>
         </is>
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>Georgia Southern -3.5</t>
+          <t>SMU -29.5</t>
         </is>
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>Georgia Southern -2.5</t>
+          <t>SMU -28.3</t>
         </is>
       </c>
       <c r="I39" t="n">
-        <v>2.5</v>
+        <v>-28.3</v>
       </c>
       <c r="J39" t="n">
-        <v>3.5</v>
-      </c>
-      <c r="K39" t="inlineStr"/>
-      <c r="L39" t="inlineStr"/>
-      <c r="M39" t="inlineStr"/>
-      <c r="N39" t="inlineStr"/>
-      <c r="O39" t="inlineStr"/>
+        <v>-29.5</v>
+      </c>
+      <c r="K39" t="n">
+        <v>-18</v>
+      </c>
+      <c r="L39" t="inlineStr">
+        <is>
+          <t>SMU -18</t>
+        </is>
+      </c>
+      <c r="M39" t="n">
+        <v>1</v>
+      </c>
+      <c r="N39" t="n">
+        <v>1</v>
+      </c>
+      <c r="O39" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="n">
@@ -2297,46 +2753,58 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Miami</t>
+          <t>Coastal Carolina</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>South Florida</t>
+          <t>East Carolina</t>
         </is>
       </c>
       <c r="D40" t="n">
-        <v>7.9</v>
+        <v>4.4</v>
       </c>
       <c r="E40" t="n">
-        <v>0.8000000000000007</v>
+        <v>1.1</v>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>Miami -15.5</t>
+          <t>Coastal Carolina -nan</t>
         </is>
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>Miami -17.5</t>
+          <t>East Carolina -7</t>
         </is>
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>Miami -18.3</t>
+          <t>East Carolina -8.1</t>
         </is>
       </c>
       <c r="I40" t="n">
-        <v>18.3</v>
+        <v>-8.1</v>
       </c>
       <c r="J40" t="n">
-        <v>17.5</v>
-      </c>
-      <c r="K40" t="inlineStr"/>
-      <c r="L40" t="inlineStr"/>
-      <c r="M40" t="inlineStr"/>
-      <c r="N40" t="inlineStr"/>
-      <c r="O40" t="inlineStr"/>
+        <v>-7</v>
+      </c>
+      <c r="K40" t="n">
+        <v>-38</v>
+      </c>
+      <c r="L40" t="inlineStr">
+        <is>
+          <t>East Carolina -38</t>
+        </is>
+      </c>
+      <c r="M40" t="n">
+        <v>1</v>
+      </c>
+      <c r="N40" t="n">
+        <v>1</v>
+      </c>
+      <c r="O40" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="n">
@@ -2344,46 +2812,58 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Missouri State</t>
+          <t>Troy</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>SMU</t>
+          <t>Memphis</t>
         </is>
       </c>
       <c r="D41" t="n">
-        <v>2</v>
+        <v>6.5</v>
       </c>
       <c r="E41" t="n">
-        <v>0.8000000000000007</v>
+        <v>0.9000000000000004</v>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>SMU -27.5</t>
+          <t>Troy -nan</t>
         </is>
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>SMU -27.5</t>
+          <t>Memphis -4.5</t>
         </is>
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>SMU -28.3</t>
+          <t>Memphis -5.4</t>
         </is>
       </c>
       <c r="I41" t="n">
-        <v>-28.3</v>
+        <v>-5.4</v>
       </c>
       <c r="J41" t="n">
-        <v>-27.5</v>
-      </c>
-      <c r="K41" t="inlineStr"/>
-      <c r="L41" t="inlineStr"/>
-      <c r="M41" t="inlineStr"/>
-      <c r="N41" t="inlineStr"/>
-      <c r="O41" t="inlineStr"/>
+        <v>-4.5</v>
+      </c>
+      <c r="K41" t="n">
+        <v>-21</v>
+      </c>
+      <c r="L41" t="inlineStr">
+        <is>
+          <t>Memphis -21</t>
+        </is>
+      </c>
+      <c r="M41" t="n">
+        <v>1</v>
+      </c>
+      <c r="N41" t="n">
+        <v>1</v>
+      </c>
+      <c r="O41" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="n">
@@ -2391,46 +2871,58 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>LSU</t>
+          <t>Illinois</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Florida</t>
+          <t>Western Michigan</t>
         </is>
       </c>
       <c r="D42" t="n">
-        <v>9.800000000000001</v>
+        <v>3.3</v>
       </c>
       <c r="E42" t="n">
-        <v>0.7999999999999998</v>
+        <v>0.8999999999999986</v>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>LSU -5.5</t>
+          <t>Illinois -nan</t>
         </is>
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>LSU -5.5</t>
+          <t>Illinois -27.5</t>
         </is>
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>LSU -6.3</t>
+          <t>Illinois -26.6</t>
         </is>
       </c>
       <c r="I42" t="n">
-        <v>6.3</v>
+        <v>26.6</v>
       </c>
       <c r="J42" t="n">
-        <v>5.5</v>
-      </c>
-      <c r="K42" t="inlineStr"/>
-      <c r="L42" t="inlineStr"/>
-      <c r="M42" t="inlineStr"/>
-      <c r="N42" t="inlineStr"/>
-      <c r="O42" t="inlineStr"/>
+        <v>27.5</v>
+      </c>
+      <c r="K42" t="n">
+        <v>38</v>
+      </c>
+      <c r="L42" t="inlineStr">
+        <is>
+          <t>Illinois -38</t>
+        </is>
+      </c>
+      <c r="M42" t="n">
+        <v>1</v>
+      </c>
+      <c r="N42" t="n">
+        <v>0</v>
+      </c>
+      <c r="O42" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="n">
@@ -2438,46 +2930,58 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Troy</t>
+          <t>Miami</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Memphis</t>
+          <t>South Florida</t>
         </is>
       </c>
       <c r="D43" t="n">
-        <v>6.5</v>
+        <v>7.9</v>
       </c>
       <c r="E43" t="n">
-        <v>0.7999999999999998</v>
+        <v>0.8999999999999986</v>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>Troy -nan</t>
+          <t>Miami -nan</t>
         </is>
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>Memphis -4.5</t>
+          <t>Miami -17.5</t>
         </is>
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>Memphis -5.3</t>
+          <t>Miami -18.4</t>
         </is>
       </c>
       <c r="I43" t="n">
-        <v>-5.3</v>
+        <v>18.4</v>
       </c>
       <c r="J43" t="n">
-        <v>-4.5</v>
-      </c>
-      <c r="K43" t="inlineStr"/>
-      <c r="L43" t="inlineStr"/>
-      <c r="M43" t="inlineStr"/>
-      <c r="N43" t="inlineStr"/>
-      <c r="O43" t="inlineStr"/>
+        <v>17.5</v>
+      </c>
+      <c r="K43" t="n">
+        <v>37</v>
+      </c>
+      <c r="L43" t="inlineStr">
+        <is>
+          <t>Miami -37</t>
+        </is>
+      </c>
+      <c r="M43" t="n">
+        <v>1</v>
+      </c>
+      <c r="N43" t="n">
+        <v>1</v>
+      </c>
+      <c r="O43" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="n">
@@ -2485,46 +2989,58 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>California</t>
+          <t>Delaware</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Minnesota</t>
+          <t>UConn</t>
         </is>
       </c>
       <c r="D44" t="n">
-        <v>8</v>
+        <v>3.4</v>
       </c>
       <c r="E44" t="n">
-        <v>0.6000000000000001</v>
+        <v>0.7999999999999998</v>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>Minnesota -2.5</t>
+          <t>Delaware -nan</t>
         </is>
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>Minnesota -2.5</t>
+          <t>UConn -8.5</t>
         </is>
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>Minnesota -1.9</t>
+          <t>UConn -7.7</t>
         </is>
       </c>
       <c r="I44" t="n">
-        <v>-1.9</v>
+        <v>-7.7</v>
       </c>
       <c r="J44" t="n">
-        <v>-2.5</v>
-      </c>
-      <c r="K44" t="inlineStr"/>
-      <c r="L44" t="inlineStr"/>
-      <c r="M44" t="inlineStr"/>
-      <c r="N44" t="inlineStr"/>
-      <c r="O44" t="inlineStr"/>
+        <v>-8.5</v>
+      </c>
+      <c r="K44" t="n">
+        <v>3</v>
+      </c>
+      <c r="L44" t="inlineStr">
+        <is>
+          <t>Delaware -3</t>
+        </is>
+      </c>
+      <c r="M44" t="n">
+        <v>1</v>
+      </c>
+      <c r="N44" t="n">
+        <v>1</v>
+      </c>
+      <c r="O44" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="n">
@@ -2532,46 +3048,58 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Texas Tech</t>
+          <t>Tennessee</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Oregon State</t>
+          <t>Georgia</t>
         </is>
       </c>
       <c r="D45" t="n">
-        <v>5.4</v>
+        <v>9.6</v>
       </c>
       <c r="E45" t="n">
-        <v>0.3000000000000007</v>
+        <v>0.7000000000000002</v>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>Texas Tech -24.5</t>
+          <t>Georgia -7.5</t>
         </is>
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>Texas Tech -23.5</t>
+          <t>Georgia -3.5</t>
         </is>
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>Texas Tech -23.2</t>
+          <t>Georgia -4.2</t>
         </is>
       </c>
       <c r="I45" t="n">
-        <v>23.2</v>
+        <v>-4.2</v>
       </c>
       <c r="J45" t="n">
-        <v>23.5</v>
-      </c>
-      <c r="K45" t="inlineStr"/>
-      <c r="L45" t="inlineStr"/>
-      <c r="M45" t="inlineStr"/>
-      <c r="N45" t="inlineStr"/>
-      <c r="O45" t="inlineStr"/>
+        <v>-3.5</v>
+      </c>
+      <c r="K45" t="n">
+        <v>-3</v>
+      </c>
+      <c r="L45" t="inlineStr">
+        <is>
+          <t>Georgia -3</t>
+        </is>
+      </c>
+      <c r="M45" t="n">
+        <v>1</v>
+      </c>
+      <c r="N45" t="n">
+        <v>0</v>
+      </c>
+      <c r="O45" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="n">
@@ -2579,46 +3107,58 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Coastal Carolina</t>
+          <t>Georgia Southern</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>East Carolina</t>
+          <t>Jacksonville State</t>
         </is>
       </c>
       <c r="D46" t="n">
-        <v>4.4</v>
+        <v>6.6</v>
       </c>
       <c r="E46" t="n">
-        <v>0.2999999999999998</v>
+        <v>0.5</v>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>East Carolina -6.5</t>
+          <t>Georgia Southern -4.0</t>
         </is>
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>East Carolina -7.5</t>
+          <t>Georgia Southern -3</t>
         </is>
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>East Carolina -7.8</t>
+          <t>Georgia Southern -2.5</t>
         </is>
       </c>
       <c r="I46" t="n">
-        <v>-7.8</v>
+        <v>2.5</v>
       </c>
       <c r="J46" t="n">
-        <v>-7.5</v>
-      </c>
-      <c r="K46" t="inlineStr"/>
-      <c r="L46" t="inlineStr"/>
-      <c r="M46" t="inlineStr"/>
-      <c r="N46" t="inlineStr"/>
-      <c r="O46" t="inlineStr"/>
+        <v>3</v>
+      </c>
+      <c r="K46" t="n">
+        <v>7</v>
+      </c>
+      <c r="L46" t="inlineStr">
+        <is>
+          <t>Georgia Southern -7</t>
+        </is>
+      </c>
+      <c r="M46" t="n">
+        <v>0</v>
+      </c>
+      <c r="N46" t="n">
+        <v>0</v>
+      </c>
+      <c r="O46" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="n">
@@ -2626,46 +3166,58 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Louisiana Tech</t>
+          <t>Bowling Green</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>New Mexico State</t>
+          <t>Liberty</t>
         </is>
       </c>
       <c r="D47" t="n">
-        <v>4.2</v>
+        <v>4.8</v>
       </c>
       <c r="E47" t="n">
-        <v>0.1999999999999993</v>
+        <v>0.2999999999999998</v>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>Louisiana Tech -12.5</t>
+          <t>Bowling Green -nan</t>
         </is>
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>Louisiana Tech -9.5</t>
+          <t>Liberty -6</t>
         </is>
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>Louisiana Tech -9.7</t>
+          <t>Liberty -6.3</t>
         </is>
       </c>
       <c r="I47" t="n">
-        <v>9.699999999999999</v>
+        <v>-6.3</v>
       </c>
       <c r="J47" t="n">
-        <v>9.5</v>
-      </c>
-      <c r="K47" t="inlineStr"/>
-      <c r="L47" t="inlineStr"/>
-      <c r="M47" t="inlineStr"/>
-      <c r="N47" t="inlineStr"/>
-      <c r="O47" t="inlineStr"/>
+        <v>-6</v>
+      </c>
+      <c r="K47" t="n">
+        <v>10</v>
+      </c>
+      <c r="L47" t="inlineStr">
+        <is>
+          <t>Bowling Green -10</t>
+        </is>
+      </c>
+      <c r="M47" t="n">
+        <v>1</v>
+      </c>
+      <c r="N47" t="n">
+        <v>0</v>
+      </c>
+      <c r="O47" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="n">
@@ -2673,46 +3225,58 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Bowling Green</t>
+          <t>Louisiana Tech</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Liberty</t>
+          <t>New Mexico State</t>
         </is>
       </c>
       <c r="D48" t="n">
-        <v>4.8</v>
+        <v>4.2</v>
       </c>
       <c r="E48" t="n">
         <v>0.09999999999999964</v>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>Liberty -7.5</t>
+          <t>Louisiana Tech -nan</t>
         </is>
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>Liberty -6.5</t>
+          <t>Louisiana Tech -10</t>
         </is>
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>Liberty -6.4</t>
+          <t>Louisiana Tech -9.9</t>
         </is>
       </c>
       <c r="I48" t="n">
-        <v>-6.4</v>
+        <v>9.9</v>
       </c>
       <c r="J48" t="n">
-        <v>-6.5</v>
-      </c>
-      <c r="K48" t="inlineStr"/>
-      <c r="L48" t="inlineStr"/>
-      <c r="M48" t="inlineStr"/>
-      <c r="N48" t="inlineStr"/>
-      <c r="O48" t="inlineStr"/>
+        <v>10</v>
+      </c>
+      <c r="K48" t="n">
+        <v>35</v>
+      </c>
+      <c r="L48" t="inlineStr">
+        <is>
+          <t>Louisiana Tech -35</t>
+        </is>
+      </c>
+      <c r="M48" t="n">
+        <v>1</v>
+      </c>
+      <c r="N48" t="n">
+        <v>0</v>
+      </c>
+      <c r="O48" t="n">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>